<commit_message>
Updated GBM sheets to current schemas.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{403EA2DA-3D41-334A-90F6-46B6AD26538F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{40FF5333-52FF-D645-9923-2905F0C75B8E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="580" windowWidth="26540" windowHeight="16580" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="508">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Tissue Stability</t>
   </si>
   <si>
-    <t>project.project_core.project_shortname</t>
-  </si>
-  <si>
     <t>Add your data below this line</t>
   </si>
   <si>
@@ -220,24 +217,6 @@
     <t>donor_organism.biomaterial_core.ncbi_taxon_id</t>
   </si>
   <si>
-    <t>Genotype of biomaterial including strain, cross, and genetic modification information.</t>
-  </si>
-  <si>
-    <t>Genotype</t>
-  </si>
-  <si>
-    <t>donor_organism.biomaterial_core.genotype</t>
-  </si>
-  <si>
-    <t>The karyotype of the biomaterial.</t>
-  </si>
-  <si>
-    <t>Karyotype</t>
-  </si>
-  <si>
-    <t>donor_organism.biomaterial_core.karyotype</t>
-  </si>
-  <si>
     <t>A list of filenames of biomaterial-level supplementary files.</t>
   </si>
   <si>
@@ -616,12 +595,6 @@
     <t>specimen_from_organism.collection_time</t>
   </si>
   <si>
-    <t>specimen_from_organism.biomaterial_core.genotype</t>
-  </si>
-  <si>
-    <t>specimen_from_organism.biomaterial_core.karyotype</t>
-  </si>
-  <si>
     <t>specimen_from_organism.biomaterial_core.supplementary_files</t>
   </si>
   <si>
@@ -736,12 +709,6 @@
     <t>cell_suspension.biomaterial_core.ncbi_taxon_id</t>
   </si>
   <si>
-    <t>cell_suspension.biomaterial_core.genotype</t>
-  </si>
-  <si>
-    <t>cell_suspension.biomaterial_core.karyotype</t>
-  </si>
-  <si>
     <t>cell_suspension.biomaterial_core.supplementary_files</t>
   </si>
   <si>
@@ -970,9 +937,6 @@
     <t>Well plate ID</t>
   </si>
   <si>
-    <t>sequence_file.smartseq2.plate_id</t>
-  </si>
-  <si>
     <t>A name for the well. Should be unique for the plate</t>
   </si>
   <si>
@@ -985,9 +949,6 @@
     <t>Cell quality</t>
   </si>
   <si>
-    <t>sequence_file.smartseq2.cell_quality</t>
-  </si>
-  <si>
     <t>library_preparation_protocol.protocol_core.protocol_id</t>
   </si>
   <si>
@@ -1585,7 +1546,13 @@
     <t>EMBL-EBI</t>
   </si>
   <si>
-    <t>sequence_file.smartseq2.well_id</t>
+    <t>cell_suspension.plate_based_sequencing.plate_id</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.well_id</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.cell_quality</t>
   </si>
 </sst>
 </file>
@@ -2016,7 +1983,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2036,25 +2003,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2062,25 +2029,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2088,55 +2055,55 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>503</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="B6" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="C6" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -2148,8 +2115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2170,155 +2137,155 @@
   <sheetData>
     <row r="1" spans="1:12" ht="90" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F3" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="I3" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="J3" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="B4" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="C4" t="s">
+        <v>438</v>
+      </c>
+      <c r="D4" t="s">
+        <v>443</v>
+      </c>
+      <c r="E4" t="s">
+        <v>444</v>
+      </c>
+      <c r="F4" t="s">
         <v>451</v>
       </c>
-      <c r="D4" t="s">
-        <v>456</v>
-      </c>
-      <c r="E4" t="s">
-        <v>457</v>
-      </c>
-      <c r="F4" t="s">
-        <v>464</v>
-      </c>
       <c r="G4" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="H4" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="I4" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="J4" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="K4" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="L4" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>476</v>
+      </c>
+      <c r="B6" t="s">
+        <v>496</v>
+      </c>
+      <c r="D6" t="s">
+        <v>477</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="F6" t="s">
+        <v>450</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>489</v>
-      </c>
-      <c r="B6" t="s">
-        <v>509</v>
-      </c>
-      <c r="D6" t="s">
-        <v>490</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>510</v>
-      </c>
-      <c r="F6" t="s">
-        <v>463</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -2331,7 +2298,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2347,25 +2314,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -2373,25 +2340,25 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>1</v>
@@ -2399,7 +2366,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
         <v>2</v>
@@ -2407,47 +2374,47 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="B6" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="D6" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="H6" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -2457,10 +2424,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AV6"/>
+  <dimension ref="A1:AT6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2472,513 +2439,493 @@
     <col min="6" max="6" width="37.6640625" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" customWidth="1"/>
-    <col min="15" max="15" width="44.6640625" customWidth="1"/>
-    <col min="16" max="17" width="48.6640625" customWidth="1"/>
-    <col min="18" max="18" width="52.6640625" customWidth="1"/>
-    <col min="19" max="20" width="14.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.6640625" customWidth="1"/>
-    <col min="22" max="22" width="20.6640625" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" customWidth="1"/>
-    <col min="25" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="17.6640625" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="44.6640625" customWidth="1"/>
+    <col min="14" max="15" width="48.6640625" customWidth="1"/>
+    <col min="16" max="16" width="52.6640625" customWidth="1"/>
+    <col min="17" max="18" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="28.6640625" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" customWidth="1"/>
+    <col min="27" max="27" width="10.6640625" customWidth="1"/>
     <col min="28" max="28" width="12.6640625" customWidth="1"/>
-    <col min="29" max="29" width="10.6640625" customWidth="1"/>
-    <col min="30" max="30" width="12.6640625" customWidth="1"/>
+    <col min="29" max="29" width="37.6640625" customWidth="1"/>
+    <col min="30" max="30" width="41.6640625" customWidth="1"/>
     <col min="31" max="31" width="37.6640625" customWidth="1"/>
     <col min="32" max="32" width="41.6640625" customWidth="1"/>
-    <col min="33" max="33" width="37.6640625" customWidth="1"/>
-    <col min="34" max="34" width="41.6640625" customWidth="1"/>
-    <col min="35" max="35" width="27.6640625" customWidth="1"/>
-    <col min="36" max="36" width="31.6640625" customWidth="1"/>
-    <col min="37" max="37" width="8.6640625" customWidth="1"/>
-    <col min="38" max="38" width="9.6640625" customWidth="1"/>
-    <col min="39" max="39" width="10.6640625" customWidth="1"/>
-    <col min="40" max="40" width="15.6640625" customWidth="1"/>
-    <col min="41" max="41" width="40.6640625" customWidth="1"/>
-    <col min="42" max="42" width="44.6640625" customWidth="1"/>
-    <col min="43" max="43" width="6.6640625" customWidth="1"/>
-    <col min="44" max="44" width="31.6640625" customWidth="1"/>
-    <col min="45" max="45" width="35.6640625" customWidth="1"/>
-    <col min="46" max="46" width="6.6640625" customWidth="1"/>
-    <col min="47" max="47" width="31.6640625" customWidth="1"/>
-    <col min="48" max="48" width="35.6640625" customWidth="1"/>
+    <col min="33" max="33" width="27.6640625" customWidth="1"/>
+    <col min="34" max="34" width="31.6640625" customWidth="1"/>
+    <col min="35" max="35" width="8.6640625" customWidth="1"/>
+    <col min="36" max="36" width="9.6640625" customWidth="1"/>
+    <col min="37" max="37" width="10.6640625" customWidth="1"/>
+    <col min="38" max="38" width="15.6640625" customWidth="1"/>
+    <col min="39" max="39" width="40.6640625" customWidth="1"/>
+    <col min="40" max="40" width="44.6640625" customWidth="1"/>
+    <col min="41" max="41" width="6.6640625" customWidth="1"/>
+    <col min="42" max="42" width="31.6640625" customWidth="1"/>
+    <col min="43" max="43" width="35.6640625" customWidth="1"/>
+    <col min="44" max="44" width="6.6640625" customWidth="1"/>
+    <col min="45" max="45" width="31.6640625" customWidth="1"/>
+    <col min="46" max="46" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="360" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" ht="360" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="AD2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q4" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="R4" t="s">
+        <v>85</v>
+      </c>
+      <c r="S4" t="s">
+        <v>88</v>
+      </c>
+      <c r="T4" t="s">
+        <v>91</v>
+      </c>
+      <c r="U4" t="s">
+        <v>94</v>
+      </c>
+      <c r="V4" t="s">
+        <v>97</v>
+      </c>
+      <c r="W4" t="s">
+        <v>100</v>
+      </c>
+      <c r="X4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>134</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AS4" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="AT4" t="s">
         <v>160</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" t="s">
-        <v>158</v>
-      </c>
-      <c r="H4" t="s">
-        <v>161</v>
-      </c>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" t="s">
-        <v>73</v>
-      </c>
-      <c r="M4" t="s">
-        <v>76</v>
-      </c>
-      <c r="N4" t="s">
-        <v>79</v>
-      </c>
-      <c r="O4" t="s">
-        <v>81</v>
-      </c>
-      <c r="P4" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>85</v>
-      </c>
-      <c r="R4" t="s">
-        <v>86</v>
-      </c>
-      <c r="S4" t="s">
-        <v>89</v>
-      </c>
-      <c r="T4" t="s">
-        <v>92</v>
-      </c>
-      <c r="U4" t="s">
-        <v>95</v>
-      </c>
-      <c r="V4" t="s">
-        <v>98</v>
-      </c>
-      <c r="W4" t="s">
-        <v>101</v>
-      </c>
-      <c r="X4" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>128</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>130</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>131</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>135</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>141</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>144</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>147</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>148</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>149</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>152</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>154</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>155</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>166</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="D6" s="3">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="F6" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="G6" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="H6" t="s">
-        <v>475</v>
-      </c>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
+        <v>462</v>
+      </c>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2988,10 +2935,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3013,389 +2960,369 @@
     <col min="17" max="17" width="70.6640625" customWidth="1"/>
     <col min="18" max="18" width="19.6640625" customWidth="1"/>
     <col min="19" max="19" width="18.6640625" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" customWidth="1"/>
-    <col min="22" max="22" width="19.6640625" customWidth="1"/>
-    <col min="23" max="23" width="12.6640625" customWidth="1"/>
-    <col min="24" max="24" width="8.6640625" customWidth="1"/>
-    <col min="25" max="25" width="15.6640625" customWidth="1"/>
-    <col min="26" max="26" width="17.6640625" customWidth="1"/>
-    <col min="27" max="27" width="11.6640625" customWidth="1"/>
-    <col min="28" max="28" width="20.6640625" customWidth="1"/>
-    <col min="29" max="29" width="13.6640625" customWidth="1"/>
-    <col min="30" max="30" width="23.6640625" customWidth="1"/>
-    <col min="31" max="31" width="17.6640625" customWidth="1"/>
-    <col min="32" max="32" width="20.6640625" customWidth="1"/>
-    <col min="33" max="33" width="10.6640625" customWidth="1"/>
-    <col min="34" max="35" width="11.6640625" customWidth="1"/>
+    <col min="20" max="20" width="19.6640625" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" customWidth="1"/>
+    <col min="23" max="23" width="15.6640625" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" customWidth="1"/>
+    <col min="25" max="25" width="11.6640625" customWidth="1"/>
+    <col min="26" max="26" width="20.6640625" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" customWidth="1"/>
+    <col min="28" max="28" width="23.6640625" customWidth="1"/>
+    <col min="29" max="29" width="17.6640625" customWidth="1"/>
+    <col min="30" max="30" width="20.6640625" customWidth="1"/>
+    <col min="31" max="31" width="10.6640625" customWidth="1"/>
+    <col min="32" max="33" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="360" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" ht="360" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="O3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" t="s">
+        <v>167</v>
+      </c>
+      <c r="I4" t="s">
+        <v>169</v>
+      </c>
+      <c r="J4" t="s">
+        <v>170</v>
+      </c>
+      <c r="K4" t="s">
+        <v>172</v>
+      </c>
+      <c r="L4" t="s">
+        <v>469</v>
+      </c>
+      <c r="M4" t="s">
+        <v>470</v>
+      </c>
+      <c r="N4" t="s">
         <v>175</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O4" t="s">
+        <v>179</v>
+      </c>
+      <c r="P4" t="s">
         <v>180</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="Q4" t="s">
+        <v>181</v>
+      </c>
+      <c r="R4" t="s">
+        <v>184</v>
+      </c>
+      <c r="S4" t="s">
+        <v>187</v>
+      </c>
+      <c r="T4" t="s">
+        <v>188</v>
+      </c>
+      <c r="U4" t="s">
         <v>189</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="AF1" s="1" t="s">
+      <c r="V4" t="s">
+        <v>190</v>
+      </c>
+      <c r="W4" t="s">
+        <v>193</v>
+      </c>
+      <c r="X4" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>202</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG4" t="s">
         <v>221</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="O3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G4" t="s">
-        <v>173</v>
-      </c>
-      <c r="H4" t="s">
-        <v>174</v>
-      </c>
-      <c r="I4" t="s">
-        <v>176</v>
-      </c>
-      <c r="J4" t="s">
-        <v>177</v>
-      </c>
-      <c r="K4" t="s">
-        <v>179</v>
-      </c>
-      <c r="L4" t="s">
-        <v>482</v>
-      </c>
-      <c r="M4" t="s">
-        <v>483</v>
-      </c>
-      <c r="N4" t="s">
-        <v>182</v>
-      </c>
-      <c r="O4" t="s">
-        <v>186</v>
-      </c>
-      <c r="P4" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>188</v>
-      </c>
-      <c r="R4" t="s">
-        <v>191</v>
-      </c>
-      <c r="S4" t="s">
-        <v>194</v>
-      </c>
-      <c r="T4" t="s">
-        <v>195</v>
-      </c>
-      <c r="U4" t="s">
-        <v>196</v>
-      </c>
-      <c r="V4" t="s">
-        <v>197</v>
-      </c>
-      <c r="W4" t="s">
-        <v>198</v>
-      </c>
-      <c r="X4" t="s">
-        <v>199</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>202</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>205</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>208</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>211</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>214</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>220</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>223</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>226</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>229</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="E6" s="3">
         <v>9606</v>
       </c>
       <c r="F6" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="G6" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="I6" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="K6" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="V6" s="3"/>
+        <v>471</v>
+      </c>
+      <c r="T6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3404,10 +3331,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3421,359 +3348,372 @@
     <col min="7" max="7" width="38.6640625" customWidth="1"/>
     <col min="8" max="8" width="39.6640625" customWidth="1"/>
     <col min="9" max="9" width="43.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="9.6640625" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" customWidth="1"/>
-    <col min="17" max="17" width="51.6640625" customWidth="1"/>
-    <col min="18" max="18" width="55.6640625" customWidth="1"/>
-    <col min="19" max="19" width="68.6640625" customWidth="1"/>
-    <col min="20" max="20" width="21.6640625" customWidth="1"/>
-    <col min="21" max="21" width="67.6640625" customWidth="1"/>
-    <col min="22" max="22" width="16.6640625" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" customWidth="1"/>
-    <col min="24" max="24" width="13.6640625" customWidth="1"/>
-    <col min="25" max="25" width="25.6640625" customWidth="1"/>
-    <col min="26" max="26" width="26.6640625" customWidth="1"/>
-    <col min="27" max="27" width="14.6640625" customWidth="1"/>
-    <col min="28" max="28" width="26.6640625" customWidth="1"/>
-    <col min="29" max="29" width="10.6640625" customWidth="1"/>
-    <col min="30" max="31" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" customWidth="1"/>
+    <col min="18" max="18" width="51.6640625" customWidth="1"/>
+    <col min="19" max="19" width="55.6640625" customWidth="1"/>
+    <col min="20" max="20" width="68.6640625" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" customWidth="1"/>
+    <col min="22" max="22" width="67.6640625" customWidth="1"/>
+    <col min="23" max="23" width="16.6640625" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="25.6640625" customWidth="1"/>
+    <col min="27" max="27" width="26.6640625" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" customWidth="1"/>
+    <col min="29" max="29" width="26.6640625" customWidth="1"/>
+    <col min="30" max="30" width="10.6640625" customWidth="1"/>
+    <col min="31" max="32" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="360" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="360" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="V2" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="Y3" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>264</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F4" t="s">
+        <v>266</v>
+      </c>
+      <c r="G4" t="s">
+        <v>267</v>
+      </c>
+      <c r="H4" t="s">
+        <v>269</v>
+      </c>
+      <c r="I4" t="s">
+        <v>270</v>
+      </c>
+      <c r="J4" t="s">
+        <v>505</v>
+      </c>
+      <c r="K4" t="s">
+        <v>506</v>
+      </c>
+      <c r="L4" t="s">
+        <v>507</v>
+      </c>
+      <c r="M4" t="s">
+        <v>226</v>
+      </c>
+      <c r="N4" t="s">
+        <v>227</v>
+      </c>
+      <c r="O4" t="s">
+        <v>228</v>
+      </c>
+      <c r="P4" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>234</v>
+      </c>
+      <c r="R4" t="s">
+        <v>235</v>
+      </c>
+      <c r="S4" t="s">
+        <v>236</v>
+      </c>
+      <c r="T4" t="s">
+        <v>238</v>
+      </c>
+      <c r="U4" t="s">
+        <v>241</v>
+      </c>
+      <c r="V4" t="s">
         <v>243</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="W4" t="s">
+        <v>246</v>
+      </c>
+      <c r="X4" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA4" t="s">
         <v>261</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB4" t="s">
         <v>265</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC4" t="s">
         <v>274</v>
       </c>
-      <c r="AB2" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="X3" t="s">
-        <v>263</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>267</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>271</v>
-      </c>
-      <c r="AA3" t="s">
+      <c r="AD4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AE4" t="s">
         <v>275</v>
       </c>
-      <c r="AB3" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D4" t="s">
-        <v>233</v>
-      </c>
-      <c r="E4" t="s">
-        <v>234</v>
-      </c>
-      <c r="F4" t="s">
-        <v>277</v>
-      </c>
-      <c r="G4" t="s">
-        <v>278</v>
-      </c>
-      <c r="H4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I4" t="s">
-        <v>281</v>
-      </c>
-      <c r="J4" t="s">
-        <v>235</v>
-      </c>
-      <c r="K4" t="s">
-        <v>236</v>
-      </c>
-      <c r="L4" t="s">
-        <v>237</v>
-      </c>
-      <c r="M4" t="s">
-        <v>238</v>
-      </c>
-      <c r="N4" t="s">
-        <v>239</v>
-      </c>
-      <c r="O4" t="s">
-        <v>242</v>
-      </c>
-      <c r="P4" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>246</v>
-      </c>
-      <c r="R4" t="s">
-        <v>247</v>
-      </c>
-      <c r="S4" t="s">
-        <v>249</v>
-      </c>
-      <c r="T4" t="s">
-        <v>252</v>
-      </c>
-      <c r="U4" t="s">
-        <v>254</v>
-      </c>
-      <c r="V4" t="s">
-        <v>257</v>
-      </c>
-      <c r="W4" t="s">
-        <v>260</v>
-      </c>
-      <c r="X4" t="s">
-        <v>264</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>268</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>272</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>276</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>285</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>226</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>286</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="E6">
         <v>9606</v>
       </c>
       <c r="F6" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="G6" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="I6" t="s">
-        <v>513</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>496</v>
+        <v>500</v>
+      </c>
+      <c r="J6">
+        <v>1001</v>
       </c>
       <c r="AE6" t="s">
-        <v>485</v>
+        <v>483</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -3786,7 +3726,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="I1" sqref="I1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3798,211 +3738,175 @@
     <col min="5" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="13" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="270" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>304</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F3" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="G3" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F4" t="s">
         <v>292</v>
       </c>
-      <c r="D4" t="s">
-        <v>295</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>296</v>
+      </c>
+      <c r="H4" t="s">
         <v>299</v>
       </c>
-      <c r="F4" t="s">
-        <v>303</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
+        <v>306</v>
+      </c>
+      <c r="M4" t="s">
         <v>307</v>
       </c>
-      <c r="H4" t="s">
-        <v>310</v>
-      </c>
-      <c r="I4" t="s">
-        <v>313</v>
-      </c>
-      <c r="J4" t="s">
-        <v>518</v>
-      </c>
-      <c r="K4" t="s">
-        <v>318</v>
-      </c>
-      <c r="L4" t="s">
-        <v>319</v>
-      </c>
-      <c r="M4" t="s">
-        <v>320</v>
-      </c>
       <c r="N4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
       <c r="B6" t="s">
+        <v>468</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>494</v>
-      </c>
       <c r="E6" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="I6">
-        <v>1001</v>
-      </c>
       <c r="L6" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="M6" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="B7" t="s">
+        <v>468</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>494</v>
-      </c>
       <c r="E7" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="I7">
-        <v>1001</v>
-      </c>
       <c r="L7" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="M7" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -4015,7 +3919,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4037,188 +3941,188 @@
     <col min="15" max="15" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="120" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="165" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G3" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="H3" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="J3" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="K3" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="L3" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="N3" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="O3" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="C4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F4" t="s">
+        <v>345</v>
+      </c>
+      <c r="G4" t="s">
+        <v>338</v>
+      </c>
+      <c r="H4" t="s">
+        <v>339</v>
+      </c>
+      <c r="I4" t="s">
+        <v>340</v>
+      </c>
+      <c r="J4" t="s">
+        <v>346</v>
+      </c>
+      <c r="K4" t="s">
+        <v>347</v>
+      </c>
+      <c r="L4" t="s">
+        <v>348</v>
+      </c>
+      <c r="M4" t="s">
         <v>350</v>
       </c>
-      <c r="D4" t="s">
-        <v>354</v>
-      </c>
-      <c r="E4" t="s">
-        <v>355</v>
-      </c>
-      <c r="F4" t="s">
-        <v>358</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="N4" t="s">
         <v>351</v>
       </c>
-      <c r="H4" t="s">
+      <c r="O4" t="s">
         <v>352</v>
-      </c>
-      <c r="I4" t="s">
-        <v>353</v>
-      </c>
-      <c r="J4" t="s">
-        <v>359</v>
-      </c>
-      <c r="K4" t="s">
-        <v>360</v>
-      </c>
-      <c r="L4" t="s">
-        <v>361</v>
-      </c>
-      <c r="M4" t="s">
-        <v>363</v>
-      </c>
-      <c r="N4" t="s">
-        <v>364</v>
-      </c>
-      <c r="O4" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="B6" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="D6" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="E6" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
       <c r="F6" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -4251,137 +4155,137 @@
   <sheetData>
     <row r="1" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F3" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="G3" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="I3" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E4" t="s">
+        <v>359</v>
+      </c>
+      <c r="F4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H4" t="s">
+        <v>357</v>
+      </c>
+      <c r="I4" t="s">
+        <v>363</v>
+      </c>
+      <c r="J4" t="s">
         <v>366</v>
       </c>
-      <c r="C4" t="s">
-        <v>367</v>
-      </c>
-      <c r="D4" t="s">
-        <v>371</v>
-      </c>
-      <c r="E4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F4" t="s">
-        <v>368</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>369</v>
-      </c>
-      <c r="H4" t="s">
-        <v>370</v>
-      </c>
-      <c r="I4" t="s">
-        <v>376</v>
-      </c>
-      <c r="J4" t="s">
-        <v>379</v>
-      </c>
-      <c r="K4" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>472</v>
+      </c>
+      <c r="B6" t="s">
+        <v>491</v>
+      </c>
+      <c r="D6" t="s">
         <v>485</v>
       </c>
-      <c r="B6" t="s">
-        <v>504</v>
-      </c>
-      <c r="D6" t="s">
-        <v>498</v>
-      </c>
       <c r="E6" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -4393,8 +4297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4444,491 +4348,491 @@
   <sheetData>
     <row r="1" spans="1:44" ht="165" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="U1" s="1"/>
       <c r="V1" s="1" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="S2" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="AG2" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="AP2" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="AH2" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>447</v>
-      </c>
       <c r="AQ2" s="2" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="J3" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="K3" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="L3" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="R3" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="S3" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="T3" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="V3" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="W3" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="X3" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="Y3" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="Z3" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="AB3" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="AC3" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="AD3" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="AE3" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="AF3" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="AH3" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="AI3" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="B4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D4" t="s">
+        <v>388</v>
+      </c>
+      <c r="E4" t="s">
+        <v>389</v>
+      </c>
+      <c r="F4" t="s">
+        <v>391</v>
+      </c>
+      <c r="G4" t="s">
+        <v>392</v>
+      </c>
+      <c r="H4" t="s">
+        <v>410</v>
+      </c>
+      <c r="I4" t="s">
+        <v>413</v>
+      </c>
+      <c r="J4" t="s">
+        <v>417</v>
+      </c>
+      <c r="K4" t="s">
+        <v>372</v>
+      </c>
+      <c r="L4" t="s">
+        <v>373</v>
+      </c>
+      <c r="M4" t="s">
+        <v>374</v>
+      </c>
+      <c r="N4" t="s">
+        <v>377</v>
+      </c>
+      <c r="O4" t="s">
+        <v>380</v>
+      </c>
+      <c r="P4" t="s">
         <v>383</v>
       </c>
-      <c r="C4" t="s">
-        <v>384</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="Q4" t="s">
+        <v>386</v>
+      </c>
+      <c r="R4" t="s">
+        <v>393</v>
+      </c>
+      <c r="S4" t="s">
+        <v>394</v>
+      </c>
+      <c r="T4" t="s">
+        <v>395</v>
+      </c>
+      <c r="U4" t="s">
+        <v>397</v>
+      </c>
+      <c r="V4" t="s">
+        <v>398</v>
+      </c>
+      <c r="W4" t="s">
+        <v>399</v>
+      </c>
+      <c r="X4" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y4" t="s">
         <v>401</v>
       </c>
-      <c r="E4" t="s">
+      <c r="Z4" t="s">
         <v>402</v>
       </c>
-      <c r="F4" t="s">
+      <c r="AA4" t="s">
         <v>404</v>
       </c>
-      <c r="G4" t="s">
+      <c r="AB4" t="s">
         <v>405</v>
       </c>
-      <c r="H4" t="s">
+      <c r="AC4" t="s">
+        <v>406</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>418</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>419</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>422</v>
+      </c>
+      <c r="AH4" t="s">
         <v>423</v>
       </c>
-      <c r="I4" t="s">
-        <v>426</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="AI4" t="s">
+        <v>424</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>427</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>428</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>429</v>
+      </c>
+      <c r="AM4" t="s">
         <v>430</v>
       </c>
-      <c r="K4" t="s">
-        <v>385</v>
-      </c>
-      <c r="L4" t="s">
-        <v>386</v>
-      </c>
-      <c r="M4" t="s">
-        <v>387</v>
-      </c>
-      <c r="N4" t="s">
-        <v>390</v>
-      </c>
-      <c r="O4" t="s">
-        <v>393</v>
-      </c>
-      <c r="P4" t="s">
-        <v>396</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>399</v>
-      </c>
-      <c r="R4" t="s">
-        <v>406</v>
-      </c>
-      <c r="S4" t="s">
-        <v>407</v>
-      </c>
-      <c r="T4" t="s">
-        <v>408</v>
-      </c>
-      <c r="U4" t="s">
-        <v>410</v>
-      </c>
-      <c r="V4" t="s">
-        <v>411</v>
-      </c>
-      <c r="W4" t="s">
-        <v>412</v>
-      </c>
-      <c r="X4" t="s">
-        <v>413</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>414</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>415</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>417</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>418</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>419</v>
-      </c>
-      <c r="AD4" t="s">
+      <c r="AN4" t="s">
         <v>431</v>
       </c>
-      <c r="AE4" t="s">
-        <v>432</v>
-      </c>
-      <c r="AF4" t="s">
+      <c r="AO4" t="s">
         <v>433</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AP4" t="s">
+        <v>434</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>435</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AR4" t="s">
         <v>436</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>437</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>440</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>441</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>442</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>443</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>444</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>446</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>447</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>448</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="B6" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="D6" t="s">
+        <v>474</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="F6" t="s">
+        <v>475</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>506</v>
-      </c>
-      <c r="F6" t="s">
-        <v>488</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>500</v>
-      </c>
       <c r="H6" s="5" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
       <c r="I6" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="J6" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed short name back to shortname in user friendly row.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{019426B7-9FB9-F248-8B03-F0271568274D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF75DDE0-5393-9D48-BD69-1CB4B985B19E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="510">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -1556,6 +1556,9 @@
   </si>
   <si>
     <t>cell_suspension.plate_based_sequencing.cell_quality</t>
+  </si>
+  <si>
+    <t>Project shortname</t>
   </si>
 </sst>
 </file>
@@ -1983,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2027,7 +2030,7 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>500</v>
+        <v>509</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -2116,7 +2119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated DCP-wide integration test spreadsheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF75DDE0-5393-9D48-BD69-1CB4B985B19E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2F151456-0E4D-D54D-ACEC-C799938F7877}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -505,9 +505,6 @@
     <t>Biological sex</t>
   </si>
   <si>
-    <t>donor_organism.biological_sex</t>
-  </si>
-  <si>
     <t>Weight of organism in kilograms.</t>
   </si>
   <si>
@@ -1393,9 +1390,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>sequencing_protocol.paired_ends</t>
-  </si>
-  <si>
     <t>The name of a sequencing approach being used.</t>
   </si>
   <si>
@@ -1559,6 +1553,12 @@
   </si>
   <si>
     <t>Project shortname</t>
+  </si>
+  <si>
+    <t>donor_organism.sex</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.paired_end</t>
   </si>
 </sst>
 </file>
@@ -1986,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2101,13 +2101,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>456</v>
+      </c>
+      <c r="B6" t="s">
+        <v>457</v>
+      </c>
+      <c r="C6" t="s">
         <v>458</v>
-      </c>
-      <c r="B6" t="s">
-        <v>459</v>
-      </c>
-      <c r="C6" t="s">
-        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -2119,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2141,37 +2141,37 @@
   <sheetData>
     <row r="1" spans="1:12" ht="90" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>79</v>
@@ -2179,89 +2179,89 @@
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>447</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C4" t="s">
         <v>440</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>441</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>442</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>443</v>
       </c>
-      <c r="F4" t="s">
-        <v>444</v>
-      </c>
       <c r="G4" t="s">
+        <v>445</v>
+      </c>
+      <c r="H4" t="s">
         <v>446</v>
       </c>
-      <c r="H4" t="s">
-        <v>447</v>
-      </c>
       <c r="I4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J4" t="s">
+        <v>509</v>
+      </c>
+      <c r="K4" t="s">
         <v>454</v>
       </c>
-      <c r="K4" t="s">
-        <v>456</v>
-      </c>
       <c r="L4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2271,19 +2271,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="J6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2360,7 @@
         <v>47</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2394,7 +2394,7 @@
         <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2404,16 +2404,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -2425,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AU6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AR5" sqref="AR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2612,10 +2612,10 @@
         <v>156</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>79</v>
@@ -2755,13 +2755,13 @@
         <v>157</v>
       </c>
       <c r="AS2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AT2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AU2" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
@@ -2895,16 +2895,16 @@
         <v>155</v>
       </c>
       <c r="AR4" t="s">
-        <v>158</v>
+        <v>508</v>
       </c>
       <c r="AS4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AT4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AU4" t="s">
         <v>163</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2914,25 +2914,25 @@
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="V6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Y6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="AQ6" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="AR6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -3009,19 +3009,19 @@
         <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>129</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>123</v>
@@ -3030,10 +3030,10 @@
         <v>79</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>129</v>
@@ -3057,37 +3057,37 @@
         <v>71</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3107,46 +3107,46 @@
         <v>59</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>62</v>
@@ -3164,149 +3164,149 @@
         <v>72</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="M3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
       </c>
       <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" t="s">
         <v>166</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>167</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>168</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>169</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>170</v>
       </c>
-      <c r="H4" t="s">
-        <v>171</v>
-      </c>
       <c r="I4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J4" t="s">
         <v>173</v>
       </c>
-      <c r="J4" t="s">
-        <v>174</v>
-      </c>
       <c r="K4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M4" t="s">
+        <v>182</v>
+      </c>
+      <c r="N4" t="s">
         <v>183</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>184</v>
       </c>
-      <c r="O4" t="s">
-        <v>185</v>
-      </c>
       <c r="P4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q4" t="s">
+        <v>190</v>
+      </c>
+      <c r="R4" t="s">
+        <v>470</v>
+      </c>
+      <c r="S4" t="s">
+        <v>471</v>
+      </c>
+      <c r="T4" t="s">
         <v>191</v>
       </c>
-      <c r="R4" t="s">
-        <v>472</v>
-      </c>
-      <c r="S4" t="s">
-        <v>473</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>192</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>193</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>194</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>195</v>
       </c>
-      <c r="X4" t="s">
-        <v>196</v>
-      </c>
       <c r="Y4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Z4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AA4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AC4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AG4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AH4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AI4" t="s">
         <v>226</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3316,37 +3316,37 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E6">
         <v>9606</v>
       </c>
       <c r="F6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I6" t="s">
+        <v>499</v>
+      </c>
+      <c r="J6" t="s">
+        <v>500</v>
+      </c>
+      <c r="K6" t="s">
         <v>501</v>
       </c>
-      <c r="J6" t="s">
-        <v>502</v>
-      </c>
-      <c r="K6" t="s">
-        <v>503</v>
-      </c>
       <c r="R6" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="V6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -3414,13 +3414,13 @@
         <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>68</v>
@@ -3429,10 +3429,10 @@
         <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>150</v>
@@ -3442,26 +3442,26 @@
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>117</v>
@@ -3470,22 +3470,22 @@
         <v>79</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3508,13 +3508,13 @@
         <v>62</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>69</v>
@@ -3523,182 +3523,182 @@
         <v>72</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="AA2" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="AB2" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="AC2" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="U3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="V3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="W3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AC3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" t="s">
         <v>228</v>
       </c>
-      <c r="B4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>229</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>230</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>231</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>504</v>
+      </c>
+      <c r="H4" t="s">
+        <v>505</v>
+      </c>
+      <c r="I4" t="s">
+        <v>506</v>
+      </c>
+      <c r="J4" t="s">
         <v>232</v>
       </c>
-      <c r="G4" t="s">
-        <v>506</v>
-      </c>
-      <c r="H4" t="s">
-        <v>507</v>
-      </c>
-      <c r="I4" t="s">
-        <v>508</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>233</v>
       </c>
-      <c r="K4" t="s">
-        <v>234</v>
-      </c>
       <c r="L4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M4" t="s">
+        <v>239</v>
+      </c>
+      <c r="N4" t="s">
         <v>240</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>241</v>
       </c>
-      <c r="O4" t="s">
-        <v>242</v>
-      </c>
       <c r="P4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="R4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="U4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="V4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="W4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X4" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y4" t="s">
         <v>271</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>272</v>
       </c>
-      <c r="Z4" t="s">
-        <v>273</v>
-      </c>
       <c r="AA4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB4" t="s">
         <v>275</v>
       </c>
-      <c r="AB4" t="s">
-        <v>276</v>
-      </c>
       <c r="AC4" t="s">
+        <v>279</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE4" t="s">
         <v>280</v>
       </c>
-      <c r="AD4" t="s">
-        <v>223</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>281</v>
-      </c>
       <c r="AF4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3708,19 +3708,19 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E6">
         <v>9606</v>
       </c>
       <c r="AE6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="AF6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -3751,118 +3751,118 @@
   <sheetData>
     <row r="1" spans="1:11" ht="270" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I4" t="s">
+        <v>309</v>
+      </c>
+      <c r="J4" t="s">
         <v>310</v>
       </c>
-      <c r="J4" t="s">
-        <v>311</v>
-      </c>
       <c r="K4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3872,54 +3872,54 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B6" t="s">
+        <v>469</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="B6" t="s">
-        <v>471</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>485</v>
-      </c>
       <c r="E6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F6" s="5">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="K6" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="B7" t="s">
+        <v>469</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="E7" t="s">
         <v>484</v>
-      </c>
-      <c r="B7" t="s">
-        <v>471</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="E7" t="s">
-        <v>486</v>
       </c>
       <c r="F7" s="5">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J7" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="K7" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -3955,155 +3955,155 @@
   <sheetData>
     <row r="1" spans="1:14" ht="165" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>346</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" t="s">
         <v>340</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>341</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>342</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>343</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>344</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>345</v>
       </c>
-      <c r="H4" t="s">
-        <v>346</v>
-      </c>
       <c r="I4" t="s">
+        <v>348</v>
+      </c>
+      <c r="J4" t="s">
         <v>349</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>350</v>
       </c>
-      <c r="K4" t="s">
-        <v>351</v>
-      </c>
       <c r="L4" t="s">
+        <v>352</v>
+      </c>
+      <c r="M4" t="s">
         <v>353</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>354</v>
-      </c>
-      <c r="N4" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4113,16 +4113,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>486</v>
+      </c>
+      <c r="B6" t="s">
+        <v>487</v>
+      </c>
+      <c r="G6" t="s">
         <v>488</v>
       </c>
-      <c r="B6" t="s">
+      <c r="H6" t="s">
         <v>489</v>
-      </c>
-      <c r="G6" t="s">
-        <v>490</v>
-      </c>
-      <c r="H6" t="s">
-        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -4155,118 +4155,118 @@
   <sheetData>
     <row r="1" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>362</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" t="s">
         <v>356</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>357</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>358</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>359</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>360</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>361</v>
       </c>
-      <c r="H4" t="s">
-        <v>362</v>
-      </c>
       <c r="I4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4276,13 +4276,13 @@
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -4346,130 +4346,130 @@
   <sheetData>
     <row r="1" spans="1:45" ht="270" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>79</v>
@@ -4477,335 +4477,335 @@
     </row>
     <row r="2" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="M2" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>395</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AP2" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="T3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="U3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="W3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Y3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Z3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AB3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AD3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AE3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AG3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AI3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AJ3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>377</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="M4" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="R4" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="W4" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="X4" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="Y4" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="Z4" s="2" t="s">
-        <v>409</v>
-      </c>
       <c r="AA4" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AD4" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="AE4" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AF4" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AG4" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="AG4" s="2" t="s">
-        <v>423</v>
-      </c>
       <c r="AH4" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="AI4" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="AI4" s="2" t="s">
+      <c r="AJ4" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="AJ4" s="2" t="s">
-        <v>427</v>
-      </c>
       <c r="AK4" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AL4" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="AL4" s="2" t="s">
+      <c r="AM4" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="AM4" s="2" t="s">
+      <c r="AN4" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="AN4" s="2" t="s">
+      <c r="AO4" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="AO4" s="2" t="s">
-        <v>434</v>
-      </c>
       <c r="AP4" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="AQ4" s="2" t="s">
+      <c r="AR4" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="AR4" s="2" t="s">
+      <c r="AS4" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="AS4" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
@@ -4815,28 +4815,28 @@
     </row>
     <row r="6" spans="1:45" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>474</v>
+      </c>
+      <c r="K6" t="s">
+        <v>475</v>
+      </c>
+      <c r="M6" t="s">
         <v>476</v>
       </c>
-      <c r="K6" t="s">
+      <c r="N6" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>495</v>
+      </c>
+      <c r="AB6" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="M6" t="s">
-        <v>478</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>497</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>479</v>
-      </c>
       <c r="AC6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="AD6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated DCP-wide integration spreadsheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3AD11063-8BF9-4E44-84F3-D31022F6A1B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2F151456-0E4D-D54D-ACEC-C799938F7877}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="6740" windowWidth="26540" windowHeight="16580" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -505,9 +505,6 @@
     <t>Biological sex</t>
   </si>
   <si>
-    <t>donor_organism.biological_sex</t>
-  </si>
-  <si>
     <t>Weight of organism in kilograms.</t>
   </si>
   <si>
@@ -1556,6 +1553,9 @@
   </si>
   <si>
     <t>Project shortname</t>
+  </si>
+  <si>
+    <t>donor_organism.sex</t>
   </si>
   <si>
     <t>sequencing_protocol.paired_end</t>
@@ -1987,7 +1987,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2101,13 +2101,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>456</v>
+      </c>
+      <c r="B6" t="s">
         <v>457</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>458</v>
-      </c>
-      <c r="C6" t="s">
-        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -2119,7 +2119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -2141,37 +2141,37 @@
   <sheetData>
     <row r="1" spans="1:12" ht="90" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>79</v>
@@ -2179,89 +2179,89 @@
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>447</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>455</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C4" t="s">
         <v>440</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>441</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>442</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>443</v>
       </c>
-      <c r="F4" t="s">
-        <v>444</v>
-      </c>
       <c r="G4" t="s">
+        <v>445</v>
+      </c>
+      <c r="H4" t="s">
         <v>446</v>
       </c>
-      <c r="H4" t="s">
-        <v>447</v>
-      </c>
       <c r="I4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J4" t="s">
         <v>509</v>
       </c>
       <c r="K4" t="s">
+        <v>454</v>
+      </c>
+      <c r="L4" t="s">
         <v>455</v>
-      </c>
-      <c r="L4" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2271,19 +2271,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>478</v>
+      </c>
+      <c r="G6" t="s">
         <v>479</v>
       </c>
-      <c r="G6" t="s">
-        <v>480</v>
-      </c>
       <c r="J6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K6" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>492</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2360,7 @@
         <v>47</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2394,7 +2394,7 @@
         <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2404,16 +2404,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>459</v>
+      </c>
+      <c r="B6" t="s">
         <v>460</v>
       </c>
-      <c r="B6" t="s">
-        <v>461</v>
-      </c>
       <c r="D6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -2425,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AU6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AR5" sqref="AR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2612,10 +2612,10 @@
         <v>156</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>79</v>
@@ -2755,13 +2755,13 @@
         <v>157</v>
       </c>
       <c r="AS2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AT2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AU2" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
@@ -2895,16 +2895,16 @@
         <v>155</v>
       </c>
       <c r="AR4" t="s">
-        <v>158</v>
+        <v>508</v>
       </c>
       <c r="AS4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AT4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AU4" t="s">
         <v>163</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2914,25 +2914,25 @@
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>461</v>
+      </c>
+      <c r="B6" t="s">
         <v>462</v>
-      </c>
-      <c r="B6" t="s">
-        <v>463</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="V6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Y6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AQ6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AR6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -3009,19 +3009,19 @@
         <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>129</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>123</v>
@@ -3030,10 +3030,10 @@
         <v>79</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>129</v>
@@ -3057,37 +3057,37 @@
         <v>71</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3107,46 +3107,46 @@
         <v>59</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>472</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>62</v>
@@ -3164,149 +3164,149 @@
         <v>72</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="M3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
       </c>
       <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" t="s">
         <v>166</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>167</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>168</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>169</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>170</v>
       </c>
-      <c r="H4" t="s">
-        <v>171</v>
-      </c>
       <c r="I4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J4" t="s">
         <v>173</v>
       </c>
-      <c r="J4" t="s">
-        <v>174</v>
-      </c>
       <c r="K4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M4" t="s">
+        <v>182</v>
+      </c>
+      <c r="N4" t="s">
         <v>183</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>184</v>
       </c>
-      <c r="O4" t="s">
-        <v>185</v>
-      </c>
       <c r="P4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q4" t="s">
+        <v>190</v>
+      </c>
+      <c r="R4" t="s">
+        <v>470</v>
+      </c>
+      <c r="S4" t="s">
+        <v>471</v>
+      </c>
+      <c r="T4" t="s">
         <v>191</v>
       </c>
-      <c r="R4" t="s">
-        <v>471</v>
-      </c>
-      <c r="S4" t="s">
-        <v>472</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>192</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>193</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>194</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>195</v>
       </c>
-      <c r="X4" t="s">
-        <v>196</v>
-      </c>
       <c r="Y4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Z4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AA4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AC4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AG4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AH4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AI4" t="s">
         <v>226</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3316,37 +3316,37 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C6" t="s">
         <v>466</v>
-      </c>
-      <c r="B6" t="s">
-        <v>462</v>
-      </c>
-      <c r="C6" t="s">
-        <v>467</v>
       </c>
       <c r="E6">
         <v>9606</v>
       </c>
       <c r="F6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I6" t="s">
+        <v>499</v>
+      </c>
+      <c r="J6" t="s">
         <v>500</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>501</v>
       </c>
-      <c r="K6" t="s">
-        <v>502</v>
-      </c>
       <c r="R6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="V6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -3414,13 +3414,13 @@
         <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>68</v>
@@ -3429,10 +3429,10 @@
         <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>150</v>
@@ -3442,26 +3442,26 @@
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>117</v>
@@ -3470,22 +3470,22 @@
         <v>79</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3508,13 +3508,13 @@
         <v>62</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>504</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>69</v>
@@ -3523,182 +3523,182 @@
         <v>72</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="AA2" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="AB2" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="AC2" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="U3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="V3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="W3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AC3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" t="s">
         <v>228</v>
       </c>
-      <c r="B4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>229</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>230</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>231</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>504</v>
+      </c>
+      <c r="H4" t="s">
+        <v>505</v>
+      </c>
+      <c r="I4" t="s">
+        <v>506</v>
+      </c>
+      <c r="J4" t="s">
         <v>232</v>
       </c>
-      <c r="G4" t="s">
-        <v>505</v>
-      </c>
-      <c r="H4" t="s">
-        <v>506</v>
-      </c>
-      <c r="I4" t="s">
-        <v>507</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>233</v>
       </c>
-      <c r="K4" t="s">
-        <v>234</v>
-      </c>
       <c r="L4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M4" t="s">
+        <v>239</v>
+      </c>
+      <c r="N4" t="s">
         <v>240</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>241</v>
       </c>
-      <c r="O4" t="s">
-        <v>242</v>
-      </c>
       <c r="P4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="R4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="U4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="V4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="W4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X4" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y4" t="s">
         <v>271</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>272</v>
       </c>
-      <c r="Z4" t="s">
-        <v>273</v>
-      </c>
       <c r="AA4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB4" t="s">
         <v>275</v>
       </c>
-      <c r="AB4" t="s">
-        <v>276</v>
-      </c>
       <c r="AC4" t="s">
+        <v>279</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE4" t="s">
         <v>280</v>
       </c>
-      <c r="AD4" t="s">
-        <v>223</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>281</v>
-      </c>
       <c r="AF4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3708,19 +3708,19 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E6">
         <v>9606</v>
       </c>
       <c r="AE6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AF6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -3751,118 +3751,118 @@
   <sheetData>
     <row r="1" spans="1:11" ht="270" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I4" t="s">
+        <v>309</v>
+      </c>
+      <c r="J4" t="s">
         <v>310</v>
       </c>
-      <c r="J4" t="s">
-        <v>311</v>
-      </c>
       <c r="K4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3872,54 +3872,54 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F6" s="5">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="B7" t="s">
+        <v>469</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="B7" t="s">
-        <v>470</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="E7" t="s">
         <v>484</v>
-      </c>
-      <c r="E7" t="s">
-        <v>485</v>
       </c>
       <c r="F7" s="5">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -3955,155 +3955,155 @@
   <sheetData>
     <row r="1" spans="1:14" ht="165" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>346</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" t="s">
         <v>340</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>341</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>342</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>343</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>344</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>345</v>
       </c>
-      <c r="H4" t="s">
-        <v>346</v>
-      </c>
       <c r="I4" t="s">
+        <v>348</v>
+      </c>
+      <c r="J4" t="s">
         <v>349</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>350</v>
       </c>
-      <c r="K4" t="s">
-        <v>351</v>
-      </c>
       <c r="L4" t="s">
+        <v>352</v>
+      </c>
+      <c r="M4" t="s">
         <v>353</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>354</v>
-      </c>
-      <c r="N4" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4113,16 +4113,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>486</v>
+      </c>
+      <c r="B6" t="s">
         <v>487</v>
       </c>
-      <c r="B6" t="s">
+      <c r="G6" t="s">
         <v>488</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>489</v>
-      </c>
-      <c r="H6" t="s">
-        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -4155,118 +4155,118 @@
   <sheetData>
     <row r="1" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>362</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" t="s">
         <v>356</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>357</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>358</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>359</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>360</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>361</v>
       </c>
-      <c r="H4" t="s">
-        <v>362</v>
-      </c>
       <c r="I4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4276,13 +4276,13 @@
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G6" t="s">
+        <v>488</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>489</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -4346,130 +4346,130 @@
   <sheetData>
     <row r="1" spans="1:45" ht="270" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>79</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>79</v>
@@ -4477,335 +4477,335 @@
     </row>
     <row r="2" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="M2" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>395</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AP2" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="T3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="U3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="W3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Y3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Z3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AB3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AD3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AE3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AG3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AI3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AJ3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>377</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="M4" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="R4" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="W4" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="X4" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="Y4" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="Z4" s="2" t="s">
-        <v>409</v>
-      </c>
       <c r="AA4" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AD4" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="AE4" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AF4" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AG4" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="AG4" s="2" t="s">
-        <v>423</v>
-      </c>
       <c r="AH4" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="AI4" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="AI4" s="2" t="s">
+      <c r="AJ4" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="AJ4" s="2" t="s">
-        <v>427</v>
-      </c>
       <c r="AK4" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AL4" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="AL4" s="2" t="s">
+      <c r="AM4" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="AM4" s="2" t="s">
+      <c r="AN4" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="AN4" s="2" t="s">
+      <c r="AO4" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="AO4" s="2" t="s">
-        <v>434</v>
-      </c>
       <c r="AP4" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="AQ4" s="2" t="s">
+      <c r="AR4" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="AR4" s="2" t="s">
+      <c r="AS4" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="AS4" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
@@ -4815,28 +4815,28 @@
     </row>
     <row r="6" spans="1:45" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>474</v>
+      </c>
+      <c r="K6" t="s">
         <v>475</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>476</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>495</v>
+      </c>
+      <c r="AB6" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="AA6" t="s">
+      <c r="AC6" t="s">
         <v>496</v>
       </c>
-      <c r="AB6" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>497</v>
-      </c>
       <c r="AD6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added master/prod dcp integration test spreadsheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/examples/spreadsheets/current/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2F151456-0E4D-D54D-ACEC-C799938F7877}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7A6DD067-5C01-7142-8849-B3E05DA6B6A1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="580" windowWidth="26540" windowHeight="16580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -23,20 +23,27 @@
     <sheet name="Enrichment protocol" sheetId="12" r:id="rId8"/>
     <sheet name="Library preparation protocol" sheetId="13" r:id="rId9"/>
     <sheet name="Sequencing protocol" sheetId="14" r:id="rId10"/>
+    <sheet name="Schemas" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="540">
   <si>
     <t>A unique label for the project.</t>
   </si>
   <si>
+    <t>Project shortname</t>
+  </si>
+  <si>
     <t>Tissue Stability</t>
   </si>
   <si>
+    <t>project.project_core.project_shortname</t>
+  </si>
+  <si>
     <t>Add your data below this line</t>
   </si>
   <si>
@@ -229,6 +236,9 @@
     <t>Karyotype</t>
   </si>
   <si>
+    <t>donor_organism.biomaterial_core.karyotype</t>
+  </si>
+  <si>
     <t>A list of filenames of biomaterial-level supplementary files.</t>
   </si>
   <si>
@@ -505,6 +515,9 @@
     <t>Biological sex</t>
   </si>
   <si>
+    <t>donor_organism.biological_sex</t>
+  </si>
+  <si>
     <t>Weight of organism in kilograms.</t>
   </si>
   <si>
@@ -727,6 +740,12 @@
     <t>cell_suspension.biomaterial_core.genotype</t>
   </si>
   <si>
+    <t>cell_suspension.biomaterial_core.karyotype</t>
+  </si>
+  <si>
+    <t>cell_suspension.biomaterial_core.supplementary_files</t>
+  </si>
+  <si>
     <t>cell_suspension.biomaterial_core.biosd_biomaterial</t>
   </si>
   <si>
@@ -949,15 +968,48 @@
     <t>An ID for the plate that the well is located on.</t>
   </si>
   <si>
+    <t>Well plate ID</t>
+  </si>
+  <si>
+    <t>sequence_file.smartseq2.plate_id</t>
+  </si>
+  <si>
     <t>A name for the well. Should be unique for the plate</t>
   </si>
   <si>
+    <t>Well name</t>
+  </si>
+  <si>
+    <t>sequence_file.smartseq2.well_name</t>
+  </si>
+  <si>
+    <t>Well row in plate.</t>
+  </si>
+  <si>
+    <t>Well row</t>
+  </si>
+  <si>
+    <t>sequence_file.smartseq2.well_row</t>
+  </si>
+  <si>
+    <t>Well column in plate.</t>
+  </si>
+  <si>
+    <t>Well column</t>
+  </si>
+  <si>
+    <t>sequence_file.smartseq2.well_column</t>
+  </si>
+  <si>
     <t>Note on how good cell looks if imaged in well before sequencing.</t>
   </si>
   <si>
     <t>Cell quality</t>
   </si>
   <si>
+    <t>sequence_file.smartseq2.cell_quality</t>
+  </si>
+  <si>
     <t>library_preparation_protocol.protocol_core.protocol_id</t>
   </si>
   <si>
@@ -1075,6 +1127,9 @@
     <t>Nucleic acid source</t>
   </si>
   <si>
+    <t>dissociation_protocol.nucleic_acid_source</t>
+  </si>
+  <si>
     <t>dissociation_protocol.protocol_reagents.retail_name</t>
   </si>
   <si>
@@ -1390,6 +1445,9 @@
     <t>yes</t>
   </si>
   <si>
+    <t>sequencing_protocol.paired_ends</t>
+  </si>
+  <si>
     <t>The name of a sequencing approach being used.</t>
   </si>
   <si>
@@ -1399,6 +1457,87 @@
     <t>sequencing_protocol.sequencing_approach.ontology</t>
   </si>
   <si>
+    <t>Schemas</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/7.0.0/collection_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/sequencing/7.0.0/sequencing_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/6.1.1/cell_suspension</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/file/6.1.1/sequence_file</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/6.1.1/protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/analysis/6.1.1/analysis_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/imaging/6.1.1/imaging_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/5.2.2/specimen_from_organism</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/5.2.1/cell_line</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/5.2.1/donor_organism</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/biomaterial/5.2.1/organoid</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/file/5.2.1/analysis_file</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/project/5.2.1/project</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/analysis/5.1.0/analysis_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/biomaterial_collection/5.1.0/collection_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/biomaterial_collection/5.1.0/dissociation_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/biomaterial_collection/5.1.0/enrichment_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/imaging/5.1.0/imaging_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/sequencing/5.1.0/library_preparation_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/sequencing/5.1.0/sequencing_process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial/5.1.0/biomaterial_collection_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/sequencing/3.0.0/library_preparation_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/process/2.1.1/process</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/2.0.0/dissociation_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/protocol/biomaterial_collection/2.0.0/enrichment_protocol</t>
+  </si>
+  <si>
+    <t>https://schema.humancellatlas.org/type/file/1.1.1/reference_file</t>
+  </si>
+  <si>
     <t>Q4_DEMO-project_PRJNA248302</t>
   </si>
   <si>
@@ -1438,6 +1577,9 @@
     <t>brain</t>
   </si>
   <si>
+    <t>astrocyte</t>
+  </si>
+  <si>
     <t>Q4_DEMO-cellsus_SAMN02797092</t>
   </si>
   <si>
@@ -1508,64 +1650,13 @@
   </si>
   <si>
     <t>EFO:0008441</t>
-  </si>
-  <si>
-    <t>project.project_core.project_short_name</t>
-  </si>
-  <si>
-    <t>library_preparation_protocol.nucleic_acid_source</t>
-  </si>
-  <si>
-    <t>single cell</t>
-  </si>
-  <si>
-    <t>poly-dT</t>
-  </si>
-  <si>
-    <t>Fake Institution</t>
-  </si>
-  <si>
-    <t>Project short name</t>
-  </si>
-  <si>
-    <t>UBERON:0000955</t>
-  </si>
-  <si>
-    <t>temporal lobe</t>
-  </si>
-  <si>
-    <t>UBERON:0001871</t>
-  </si>
-  <si>
-    <t>Plate ID</t>
-  </si>
-  <si>
-    <t>Well ID</t>
-  </si>
-  <si>
-    <t>cell_suspension.plate_based_sequencing.plate_id</t>
-  </si>
-  <si>
-    <t>cell_suspension.plate_based_sequencing.well_id</t>
-  </si>
-  <si>
-    <t>cell_suspension.plate_based_sequencing.cell_quality</t>
-  </si>
-  <si>
-    <t>Project shortname</t>
-  </si>
-  <si>
-    <t>donor_organism.sex</t>
-  </si>
-  <si>
-    <t>sequencing_protocol.paired_end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1589,8 +1680,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1607,12 +1711,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1630,24 +1740,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1987,7 +2105,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2007,107 +2125,107 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>493</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>456</v>
+        <v>502</v>
       </c>
       <c r="B6" t="s">
-        <v>457</v>
+        <v>503</v>
       </c>
       <c r="C6" t="s">
-        <v>458</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -2119,8 +2237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2141,152 +2259,328 @@
   <sheetData>
     <row r="1" spans="1:12" ht="90" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>444</v>
+        <v>462</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>447</v>
+        <v>465</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>450</v>
+        <v>468</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>453</v>
+        <v>472</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>323</v>
+        <v>228</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>340</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>448</v>
+        <v>463</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>466</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>451</v>
+        <v>469</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>455</v>
+        <v>473</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>318</v>
+        <v>335</v>
       </c>
       <c r="E3" t="s">
-        <v>321</v>
+        <v>338</v>
       </c>
       <c r="J3" t="s">
-        <v>452</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="B4" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="C4" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D4" t="s">
-        <v>441</v>
+        <v>459</v>
       </c>
       <c r="E4" t="s">
-        <v>442</v>
+        <v>460</v>
       </c>
       <c r="F4" t="s">
-        <v>443</v>
+        <v>461</v>
       </c>
       <c r="G4" t="s">
-        <v>445</v>
+        <v>463</v>
       </c>
       <c r="H4" t="s">
-        <v>446</v>
+        <v>464</v>
       </c>
       <c r="I4" t="s">
-        <v>449</v>
+        <v>467</v>
       </c>
       <c r="J4" t="s">
-        <v>509</v>
+        <v>471</v>
       </c>
       <c r="K4" t="s">
-        <v>454</v>
+        <v>473</v>
       </c>
       <c r="L4" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>525</v>
+      </c>
+      <c r="G6" t="s">
+        <v>526</v>
+      </c>
+      <c r="J6" t="s">
+        <v>470</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>538</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>539</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="J6" t="s">
-        <v>452</v>
-      </c>
-      <c r="K6" s="7" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="L6" s="7" t="s">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>492</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>501</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0F00-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0F00-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0F00-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0F00-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0F00-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0F00-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0F00-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0F00-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0F00-00000A000000}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{00000000-0004-0000-0F00-00000B000000}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{00000000-0004-0000-0F00-00000C000000}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{00000000-0004-0000-0F00-00000D000000}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{00000000-0004-0000-0F00-00000E000000}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{00000000-0004-0000-0F00-00000F000000}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{00000000-0004-0000-0F00-000010000000}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{00000000-0004-0000-0F00-000011000000}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{00000000-0004-0000-0F00-000012000000}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{00000000-0004-0000-0F00-000013000000}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{00000000-0004-0000-0F00-000014000000}"/>
+    <hyperlink ref="A23" r:id="rId22" xr:uid="{00000000-0004-0000-0F00-000015000000}"/>
+    <hyperlink ref="A24" r:id="rId23" xr:uid="{00000000-0004-0000-0F00-000016000000}"/>
+    <hyperlink ref="A25" r:id="rId24" xr:uid="{00000000-0004-0000-0F00-000017000000}"/>
+    <hyperlink ref="A26" r:id="rId25" xr:uid="{00000000-0004-0000-0F00-000018000000}"/>
+    <hyperlink ref="A27" r:id="rId26" xr:uid="{00000000-0004-0000-0F00-000019000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2296,7 +2590,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2304,116 +2598,112 @@
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="6" max="7" width="7.6640625" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>47</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>498</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>459</v>
+        <v>505</v>
       </c>
       <c r="B6" t="s">
-        <v>460</v>
-      </c>
-      <c r="D6" t="s">
-        <v>497</v>
+        <v>506</v>
       </c>
       <c r="H6" t="s">
-        <v>456</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -2423,82 +2713,83 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AU6"/>
+  <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="44.6640625" customWidth="1"/>
-    <col min="11" max="12" width="48.6640625" customWidth="1"/>
-    <col min="13" max="13" width="52.6640625" customWidth="1"/>
-    <col min="14" max="15" width="14.6640625" customWidth="1"/>
-    <col min="16" max="16" width="28.6640625" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" customWidth="1"/>
-    <col min="21" max="21" width="17.6640625" customWidth="1"/>
-    <col min="22" max="22" width="15.6640625" customWidth="1"/>
-    <col min="23" max="23" width="12.6640625" customWidth="1"/>
-    <col min="24" max="24" width="10.6640625" customWidth="1"/>
-    <col min="25" max="25" width="33.6640625" customWidth="1"/>
-    <col min="26" max="26" width="37.6640625" customWidth="1"/>
-    <col min="27" max="27" width="12.6640625" customWidth="1"/>
-    <col min="28" max="28" width="37.6640625" customWidth="1"/>
-    <col min="29" max="29" width="41.6640625" customWidth="1"/>
-    <col min="30" max="30" width="37.6640625" customWidth="1"/>
-    <col min="31" max="31" width="41.6640625" customWidth="1"/>
-    <col min="32" max="32" width="27.6640625" customWidth="1"/>
-    <col min="33" max="33" width="31.6640625" customWidth="1"/>
-    <col min="34" max="34" width="8.6640625" customWidth="1"/>
-    <col min="35" max="35" width="9.6640625" customWidth="1"/>
-    <col min="36" max="36" width="10.6640625" customWidth="1"/>
-    <col min="37" max="37" width="15.6640625" customWidth="1"/>
-    <col min="38" max="38" width="40.6640625" customWidth="1"/>
-    <col min="39" max="39" width="44.6640625" customWidth="1"/>
-    <col min="40" max="40" width="6.6640625" customWidth="1"/>
-    <col min="41" max="41" width="31.6640625" customWidth="1"/>
-    <col min="42" max="42" width="35.6640625" customWidth="1"/>
-    <col min="43" max="43" width="10.6640625" customWidth="1"/>
-    <col min="44" max="44" width="14.6640625" customWidth="1"/>
-    <col min="45" max="45" width="6.6640625" customWidth="1"/>
-    <col min="46" max="46" width="31.6640625" customWidth="1"/>
-    <col min="47" max="47" width="35.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="44.6640625" customWidth="1"/>
+    <col min="12" max="13" width="48.6640625" customWidth="1"/>
+    <col min="14" max="14" width="52.6640625" customWidth="1"/>
+    <col min="15" max="16" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="28.6640625" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" customWidth="1"/>
+    <col min="22" max="22" width="17.6640625" customWidth="1"/>
+    <col min="23" max="23" width="15.6640625" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" customWidth="1"/>
+    <col min="25" max="25" width="10.6640625" customWidth="1"/>
+    <col min="26" max="26" width="33.6640625" customWidth="1"/>
+    <col min="27" max="27" width="37.6640625" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" customWidth="1"/>
+    <col min="29" max="29" width="37.6640625" customWidth="1"/>
+    <col min="30" max="30" width="41.6640625" customWidth="1"/>
+    <col min="31" max="31" width="37.6640625" customWidth="1"/>
+    <col min="32" max="32" width="41.6640625" customWidth="1"/>
+    <col min="33" max="33" width="27.6640625" customWidth="1"/>
+    <col min="34" max="34" width="31.6640625" customWidth="1"/>
+    <col min="35" max="35" width="8.6640625" customWidth="1"/>
+    <col min="36" max="36" width="9.6640625" customWidth="1"/>
+    <col min="37" max="37" width="10.6640625" customWidth="1"/>
+    <col min="38" max="38" width="15.6640625" customWidth="1"/>
+    <col min="39" max="39" width="40.6640625" customWidth="1"/>
+    <col min="40" max="40" width="44.6640625" customWidth="1"/>
+    <col min="41" max="41" width="6.6640625" customWidth="1"/>
+    <col min="42" max="42" width="31.6640625" customWidth="1"/>
+    <col min="43" max="43" width="35.6640625" customWidth="1"/>
+    <col min="44" max="44" width="10.6640625" customWidth="1"/>
+    <col min="45" max="45" width="14.6640625" customWidth="1"/>
+    <col min="46" max="46" width="6.6640625" customWidth="1"/>
+    <col min="47" max="47" width="31.6640625" customWidth="1"/>
+    <col min="48" max="48" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="180" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" ht="360" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>71</v>
@@ -2510,16 +2801,16 @@
         <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>87</v>
@@ -2555,31 +2846,31 @@
         <v>117</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>123</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>136</v>
@@ -2591,197 +2882,203 @@
         <v>142</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>150</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>78</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="N2" s="2" t="s">
         <v>85</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Y2" s="3" t="s">
         <v>118</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AA2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>124</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AD2" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="AD2" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="AE2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF2" s="2" t="s">
         <v>130</v>
       </c>
+      <c r="AF2" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="AG2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AI2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AI2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AK2" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>145</v>
+      <c r="AL2" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AN2" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AN2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AO2" s="3" t="s">
         <v>151</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
         <v>154</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>157</v>
       </c>
       <c r="AS2" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
         <v>70</v>
@@ -2793,16 +3090,16 @@
         <v>76</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="N4" t="s">
         <v>86</v>
@@ -2838,31 +3135,31 @@
         <v>116</v>
       </c>
       <c r="Y4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Z4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AA4" t="s">
         <v>122</v>
       </c>
       <c r="AB4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AC4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AD4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AE4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AF4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AG4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AH4" t="s">
         <v>135</v>
@@ -2877,62 +3174,66 @@
         <v>144</v>
       </c>
       <c r="AL4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AM4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AN4" t="s">
         <v>149</v>
       </c>
       <c r="AO4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AP4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AQ4" t="s">
         <v>155</v>
       </c>
       <c r="AR4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="AS4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>162</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>461</v>
-      </c>
-      <c r="B6" t="s">
-        <v>462</v>
-      </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>9606</v>
       </c>
-      <c r="V6" t="s">
-        <v>452</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>464</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>480</v>
+      <c r="W6" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="X6" s="5"/>
+      <c r="Z6" s="6" t="s">
+        <v>510</v>
       </c>
       <c r="AR6" t="s">
-        <v>463</v>
+        <v>527</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -2945,7 +3246,7 @@
   <dimension ref="A1:AI6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2985,382 +3286,375 @@
   <sheetData>
     <row r="1" spans="1:35" ht="360" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="J2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="L2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="P2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="X2" s="2" t="s">
+      <c r="U2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>218</v>
+      <c r="X2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="M3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F4" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H4" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="I4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="J4" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="K4" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="L4" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="M4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="N4" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="O4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="P4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="Q4" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="R4" t="s">
-        <v>470</v>
+        <v>517</v>
       </c>
       <c r="S4" t="s">
-        <v>471</v>
+        <v>518</v>
       </c>
       <c r="T4" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="U4" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="V4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="W4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="X4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="Y4" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="Z4" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="AA4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AB4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="AC4" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="AD4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="AE4" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="AF4" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="AG4" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="AH4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="AI4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>465</v>
-      </c>
-      <c r="B6" t="s">
-        <v>461</v>
-      </c>
-      <c r="C6" t="s">
-        <v>466</v>
-      </c>
-      <c r="E6">
+      <c r="A6" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="E6" s="5">
         <v>9606</v>
       </c>
-      <c r="F6" t="s">
-        <v>464</v>
-      </c>
-      <c r="H6" t="s">
-        <v>468</v>
-      </c>
-      <c r="I6" t="s">
-        <v>499</v>
-      </c>
-      <c r="J6" t="s">
-        <v>500</v>
-      </c>
-      <c r="K6" t="s">
-        <v>501</v>
-      </c>
-      <c r="R6" t="s">
-        <v>472</v>
-      </c>
-      <c r="V6" t="s">
-        <v>467</v>
+      <c r="F6" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3369,358 +3663,351 @@
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="9" width="8.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="51.6640625" customWidth="1"/>
-    <col min="15" max="15" width="55.6640625" customWidth="1"/>
-    <col min="16" max="16" width="68.6640625" customWidth="1"/>
-    <col min="17" max="17" width="21.6640625" customWidth="1"/>
-    <col min="18" max="18" width="67.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16.6640625" customWidth="1"/>
-    <col min="20" max="20" width="14.6640625" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" customWidth="1"/>
-    <col min="22" max="22" width="25.6640625" customWidth="1"/>
-    <col min="23" max="23" width="26.6640625" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" customWidth="1"/>
-    <col min="25" max="25" width="34.6640625" customWidth="1"/>
-    <col min="26" max="26" width="38.6640625" customWidth="1"/>
-    <col min="27" max="27" width="39.6640625" customWidth="1"/>
-    <col min="28" max="28" width="43.6640625" customWidth="1"/>
-    <col min="29" max="29" width="26.6640625" customWidth="1"/>
-    <col min="30" max="30" width="10.6640625" customWidth="1"/>
-    <col min="31" max="32" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="51.6640625" customWidth="1"/>
+    <col min="14" max="14" width="55.6640625" customWidth="1"/>
+    <col min="15" max="15" width="68.6640625" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" customWidth="1"/>
+    <col min="17" max="17" width="67.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" customWidth="1"/>
+    <col min="21" max="21" width="25.6640625" customWidth="1"/>
+    <col min="22" max="22" width="26.6640625" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" customWidth="1"/>
+    <col min="24" max="24" width="34.6640625" customWidth="1"/>
+    <col min="25" max="25" width="38.6640625" customWidth="1"/>
+    <col min="26" max="26" width="39.6640625" customWidth="1"/>
+    <col min="27" max="27" width="43.6640625" customWidth="1"/>
+    <col min="28" max="28" width="26.6640625" customWidth="1"/>
+    <col min="29" max="29" width="10.6640625" customWidth="1"/>
+    <col min="30" max="31" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="360" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="360" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="T3" t="s">
+        <v>263</v>
+      </c>
+      <c r="U3" t="s">
+        <v>267</v>
+      </c>
+      <c r="V3" t="s">
+        <v>271</v>
+      </c>
+      <c r="W3" t="s">
+        <v>275</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E4" t="s">
         <v>234</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="F4" t="s">
+        <v>235</v>
+      </c>
+      <c r="G4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H4" t="s">
         <v>237</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1" t="s">
+      <c r="I4" t="s">
+        <v>238</v>
+      </c>
+      <c r="J4" t="s">
+        <v>239</v>
+      </c>
+      <c r="K4" t="s">
+        <v>242</v>
+      </c>
+      <c r="L4" t="s">
+        <v>245</v>
+      </c>
+      <c r="M4" t="s">
+        <v>246</v>
+      </c>
+      <c r="N4" t="s">
+        <v>247</v>
+      </c>
+      <c r="O4" t="s">
         <v>249</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="P4" t="s">
         <v>252</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC1" s="1" t="s">
+      <c r="Q4" t="s">
+        <v>254</v>
+      </c>
+      <c r="R4" t="s">
+        <v>257</v>
+      </c>
+      <c r="S4" t="s">
+        <v>260</v>
+      </c>
+      <c r="T4" t="s">
+        <v>264</v>
+      </c>
+      <c r="U4" t="s">
+        <v>268</v>
+      </c>
+      <c r="V4" t="s">
+        <v>272</v>
+      </c>
+      <c r="W4" t="s">
         <v>276</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+      <c r="X4" t="s">
         <v>277</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="U3" t="s">
-        <v>257</v>
-      </c>
-      <c r="V3" t="s">
-        <v>261</v>
-      </c>
-      <c r="W3" t="s">
-        <v>265</v>
-      </c>
-      <c r="X3" t="s">
-        <v>269</v>
-      </c>
-      <c r="AC3" t="s">
+      <c r="Y4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>227</v>
-      </c>
-      <c r="B4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D4" t="s">
-        <v>229</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="Z4" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>281</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>285</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>286</v>
+      </c>
+      <c r="AE4" t="s">
         <v>230</v>
       </c>
-      <c r="F4" t="s">
-        <v>231</v>
-      </c>
-      <c r="G4" t="s">
-        <v>504</v>
-      </c>
-      <c r="H4" t="s">
-        <v>505</v>
-      </c>
-      <c r="I4" t="s">
-        <v>506</v>
-      </c>
-      <c r="J4" t="s">
-        <v>232</v>
-      </c>
-      <c r="K4" t="s">
-        <v>233</v>
-      </c>
-      <c r="L4" t="s">
-        <v>236</v>
-      </c>
-      <c r="M4" t="s">
-        <v>239</v>
-      </c>
-      <c r="N4" t="s">
-        <v>240</v>
-      </c>
-      <c r="O4" t="s">
-        <v>241</v>
-      </c>
-      <c r="P4" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>246</v>
-      </c>
-      <c r="R4" t="s">
-        <v>248</v>
-      </c>
-      <c r="S4" t="s">
-        <v>251</v>
-      </c>
-      <c r="T4" t="s">
-        <v>254</v>
-      </c>
-      <c r="U4" t="s">
-        <v>258</v>
-      </c>
-      <c r="V4" t="s">
-        <v>262</v>
-      </c>
-      <c r="W4" t="s">
-        <v>266</v>
-      </c>
-      <c r="X4" t="s">
-        <v>270</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>271</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>272</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>274</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>275</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>279</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>222</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>280</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>469</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>465</v>
+        <v>516</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>511</v>
       </c>
       <c r="E6">
         <v>9606</v>
       </c>
+      <c r="AD6" t="s">
+        <v>533</v>
+      </c>
       <c r="AE6" t="s">
-        <v>486</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>473</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -3730,10 +4017,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3745,181 +4032,231 @@
     <col min="5" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" customWidth="1"/>
-    <col min="9" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="270" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="270" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
         <v>298</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="F3" t="s">
         <v>302</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D4" t="s">
         <v>295</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="E4" t="s">
         <v>299</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="F4" t="s">
         <v>303</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E3" t="s">
-        <v>292</v>
-      </c>
-      <c r="F3" t="s">
-        <v>296</v>
-      </c>
-      <c r="G3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>283</v>
-      </c>
-      <c r="B4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C4" t="s">
-        <v>286</v>
-      </c>
-      <c r="D4" t="s">
-        <v>289</v>
-      </c>
-      <c r="E4" t="s">
-        <v>293</v>
-      </c>
-      <c r="F4" t="s">
-        <v>297</v>
-      </c>
       <c r="G4" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="H4" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="I4" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="J4" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="K4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>481</v>
+        <v>319</v>
+      </c>
+      <c r="L4" t="s">
+        <v>322</v>
+      </c>
+      <c r="M4" t="s">
+        <v>325</v>
+      </c>
+      <c r="N4" t="s">
+        <v>326</v>
+      </c>
+      <c r="O4" t="s">
+        <v>327</v>
+      </c>
+      <c r="P4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>528</v>
       </c>
       <c r="B6" t="s">
-        <v>469</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>483</v>
+        <v>516</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>530</v>
       </c>
       <c r="E6" t="s">
-        <v>292</v>
-      </c>
-      <c r="F6" s="5">
+        <v>298</v>
+      </c>
+      <c r="F6" s="8">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
-        <v>474</v>
-      </c>
-      <c r="J6" t="s">
-        <v>478</v>
-      </c>
-      <c r="K6" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>482</v>
+      <c r="N6" t="s">
+        <v>521</v>
+      </c>
+      <c r="O6" t="s">
+        <v>525</v>
+      </c>
+      <c r="P6" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>529</v>
       </c>
       <c r="B7" t="s">
-        <v>469</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>483</v>
+        <v>516</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>530</v>
       </c>
       <c r="E7" t="s">
-        <v>484</v>
-      </c>
-      <c r="F7" s="5">
+        <v>531</v>
+      </c>
+      <c r="F7" s="8">
         <v>1</v>
       </c>
-      <c r="I7" t="s">
-        <v>474</v>
-      </c>
-      <c r="J7" t="s">
-        <v>478</v>
-      </c>
-      <c r="K7" t="s">
-        <v>485</v>
+      <c r="N7" t="s">
+        <v>521</v>
+      </c>
+      <c r="O7" t="s">
+        <v>525</v>
+      </c>
+      <c r="P7" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -3929,10 +4266,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3945,184 +4282,194 @@
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="46.6640625" customWidth="1"/>
     <col min="8" max="8" width="50.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="64.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="64.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="165" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="165" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>324</v>
+        <v>341</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="L2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>335</v>
+      </c>
+      <c r="E3" t="s">
+        <v>338</v>
+      </c>
+      <c r="J3" t="s">
         <v>344</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>318</v>
-      </c>
-      <c r="E3" t="s">
-        <v>321</v>
-      </c>
-      <c r="I3" t="s">
-        <v>327</v>
-      </c>
-      <c r="J3" t="s">
-        <v>329</v>
-      </c>
       <c r="K3" t="s">
-        <v>332</v>
-      </c>
-      <c r="M3" t="s">
-        <v>335</v>
+        <v>346</v>
+      </c>
+      <c r="L3" t="s">
+        <v>349</v>
       </c>
       <c r="N3" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+      <c r="O3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s">
-        <v>339</v>
+        <v>356</v>
       </c>
       <c r="C4" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="D4" t="s">
-        <v>341</v>
+        <v>358</v>
       </c>
       <c r="E4" t="s">
-        <v>342</v>
+        <v>359</v>
       </c>
       <c r="F4" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="G4" t="s">
-        <v>344</v>
+        <v>361</v>
       </c>
       <c r="H4" t="s">
-        <v>345</v>
+        <v>362</v>
       </c>
       <c r="I4" t="s">
-        <v>348</v>
+        <v>365</v>
       </c>
       <c r="J4" t="s">
-        <v>349</v>
+        <v>366</v>
       </c>
       <c r="K4" t="s">
-        <v>350</v>
+        <v>367</v>
       </c>
       <c r="L4" t="s">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="M4" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="N4" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+      <c r="O4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>486</v>
+        <v>533</v>
       </c>
       <c r="B6" t="s">
-        <v>487</v>
+        <v>534</v>
       </c>
       <c r="G6" t="s">
-        <v>488</v>
-      </c>
-      <c r="H6" t="s">
-        <v>489</v>
+        <v>535</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -4136,7 +4483,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4155,134 +4502,134 @@
   <sheetData>
     <row r="1" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>324</v>
+        <v>341</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>362</v>
+        <v>380</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>366</v>
+        <v>384</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>323</v>
+        <v>228</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>340</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>370</v>
+        <v>378</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>318</v>
+        <v>335</v>
       </c>
       <c r="E3" t="s">
-        <v>321</v>
+        <v>338</v>
       </c>
       <c r="I3" t="s">
-        <v>364</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B4" t="s">
-        <v>355</v>
+        <v>373</v>
       </c>
       <c r="C4" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="D4" t="s">
-        <v>357</v>
+        <v>375</v>
       </c>
       <c r="E4" t="s">
-        <v>358</v>
+        <v>376</v>
       </c>
       <c r="F4" t="s">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="G4" t="s">
-        <v>360</v>
+        <v>378</v>
       </c>
       <c r="H4" t="s">
-        <v>361</v>
+        <v>379</v>
       </c>
       <c r="I4" t="s">
-        <v>365</v>
+        <v>383</v>
       </c>
       <c r="J4" t="s">
-        <v>368</v>
+        <v>386</v>
       </c>
       <c r="K4" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>473</v>
+        <v>520</v>
       </c>
       <c r="G6" t="s">
-        <v>488</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>489</v>
+        <v>535</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -4292,10 +4639,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:AS6"/>
+  <dimension ref="A1:AR6"/>
   <sheetViews>
     <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="X4" sqref="A4:XFD4"/>
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4325,518 +4672,502 @@
     <col min="24" max="24" width="81.6640625" customWidth="1"/>
     <col min="25" max="25" width="11.6640625" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" customWidth="1"/>
-    <col min="27" max="27" width="19.6640625" customWidth="1"/>
-    <col min="28" max="28" width="8.6640625" customWidth="1"/>
-    <col min="29" max="30" width="6.6640625" customWidth="1"/>
-    <col min="31" max="31" width="11.6640625" customWidth="1"/>
-    <col min="32" max="32" width="14.6640625" customWidth="1"/>
-    <col min="33" max="33" width="12.6640625" customWidth="1"/>
-    <col min="34" max="34" width="66.6640625" customWidth="1"/>
-    <col min="35" max="35" width="11.6640625" customWidth="1"/>
-    <col min="36" max="36" width="9.6640625" customWidth="1"/>
-    <col min="37" max="37" width="17.6640625" customWidth="1"/>
-    <col min="38" max="38" width="23.6640625" customWidth="1"/>
-    <col min="39" max="40" width="14.6640625" customWidth="1"/>
-    <col min="41" max="41" width="23.6640625" customWidth="1"/>
-    <col min="42" max="42" width="65.6640625" customWidth="1"/>
-    <col min="43" max="43" width="69.6640625" customWidth="1"/>
-    <col min="44" max="44" width="67.6640625" customWidth="1"/>
-    <col min="45" max="45" width="71.6640625" customWidth="1"/>
+    <col min="27" max="27" width="8.6640625" customWidth="1"/>
+    <col min="28" max="29" width="6.6640625" customWidth="1"/>
+    <col min="30" max="30" width="11.6640625" customWidth="1"/>
+    <col min="31" max="31" width="14.6640625" customWidth="1"/>
+    <col min="32" max="32" width="12.6640625" customWidth="1"/>
+    <col min="33" max="33" width="66.6640625" customWidth="1"/>
+    <col min="34" max="34" width="11.6640625" customWidth="1"/>
+    <col min="35" max="35" width="9.6640625" customWidth="1"/>
+    <col min="36" max="36" width="17.6640625" customWidth="1"/>
+    <col min="37" max="37" width="23.6640625" customWidth="1"/>
+    <col min="38" max="39" width="14.6640625" customWidth="1"/>
+    <col min="40" max="40" width="23.6640625" customWidth="1"/>
+    <col min="41" max="41" width="65.6640625" customWidth="1"/>
+    <col min="42" max="42" width="69.6640625" customWidth="1"/>
+    <col min="43" max="43" width="67.6640625" customWidth="1"/>
+    <col min="44" max="44" width="71.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="270" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" ht="270" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>377</v>
+        <v>395</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>383</v>
+        <v>401</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>392</v>
+        <v>410</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>325</v>
+        <v>342</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>330</v>
+        <v>347</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1" t="s">
-        <v>333</v>
+        <v>350</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>336</v>
+        <v>353</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>325</v>
+        <v>342</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>330</v>
+        <v>347</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1" t="s">
-        <v>333</v>
+        <v>350</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>336</v>
+        <v>353</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>335</v>
+      </c>
+      <c r="E3" t="s">
+        <v>338</v>
+      </c>
+      <c r="O3" t="s">
+        <v>344</v>
+      </c>
+      <c r="P3" t="s">
         <v>346</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="Q3" t="s">
+        <v>349</v>
+      </c>
+      <c r="S3" t="s">
+        <v>352</v>
+      </c>
+      <c r="T3" t="s">
+        <v>355</v>
+      </c>
+      <c r="U3" t="s">
+        <v>344</v>
+      </c>
+      <c r="V3" t="s">
+        <v>346</v>
+      </c>
+      <c r="W3" t="s">
+        <v>349</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>355</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>429</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>436</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>344</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>346</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>349</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>352</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" t="s">
+        <v>390</v>
+      </c>
+      <c r="C4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D4" t="s">
+        <v>392</v>
+      </c>
+      <c r="E4" t="s">
+        <v>393</v>
+      </c>
+      <c r="F4" t="s">
+        <v>394</v>
+      </c>
+      <c r="G4" t="s">
+        <v>397</v>
+      </c>
+      <c r="H4" t="s">
+        <v>400</v>
+      </c>
+      <c r="I4" t="s">
+        <v>403</v>
+      </c>
+      <c r="J4" t="s">
+        <v>406</v>
+      </c>
+      <c r="K4" t="s">
+        <v>408</v>
+      </c>
+      <c r="L4" t="s">
         <v>409</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="M4" t="s">
+        <v>411</v>
+      </c>
+      <c r="N4" t="s">
+        <v>412</v>
+      </c>
+      <c r="O4" t="s">
         <v>413</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+      <c r="P4" t="s">
         <v>414</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="Q4" t="s">
+        <v>415</v>
+      </c>
+      <c r="R4" t="s">
         <v>417</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="S4" t="s">
+        <v>418</v>
+      </c>
+      <c r="T4" t="s">
+        <v>419</v>
+      </c>
+      <c r="U4" t="s">
+        <v>420</v>
+      </c>
+      <c r="V4" t="s">
+        <v>421</v>
+      </c>
+      <c r="W4" t="s">
+        <v>422</v>
+      </c>
+      <c r="X4" t="s">
+        <v>424</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>425</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>426</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>430</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>433</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>437</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>438</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>439</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>440</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>442</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>443</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>444</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>447</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>448</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>449</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>450</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>451</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>453</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>454</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>455</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>521</v>
+      </c>
+      <c r="K6" t="s">
+        <v>522</v>
+      </c>
+      <c r="M6" t="s">
+        <v>523</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>537</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="AC6" t="s">
         <v>436</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>318</v>
-      </c>
-      <c r="E3" t="s">
-        <v>321</v>
-      </c>
-      <c r="O3" t="s">
-        <v>327</v>
-      </c>
-      <c r="P3" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>332</v>
-      </c>
-      <c r="S3" t="s">
-        <v>335</v>
-      </c>
-      <c r="T3" t="s">
-        <v>338</v>
-      </c>
-      <c r="U3" t="s">
-        <v>327</v>
-      </c>
-      <c r="V3" t="s">
-        <v>329</v>
-      </c>
-      <c r="W3" t="s">
-        <v>332</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>335</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>338</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>411</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>418</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>327</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>329</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>332</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>335</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="AO4" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="AP4" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="AQ4" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="AR4" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="AS4" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>474</v>
-      </c>
-      <c r="K6" t="s">
-        <v>475</v>
-      </c>
-      <c r="M6" t="s">
-        <v>476</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>490</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>495</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>496</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated DCP-wide integration test SS2 sheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2F151456-0E4D-D54D-ACEC-C799938F7877}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D00E996-D753-8843-AA06-B49F9C757DCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="26540" windowHeight="16580" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1441,12 +1441,6 @@
     <t>Q4_DEMO-cellsus_SAMN02797092</t>
   </si>
   <si>
-    <t>specimen_from_organism.disease.text</t>
-  </si>
-  <si>
-    <t>specimen_from_organism.disease.ontology</t>
-  </si>
-  <si>
     <t>glioblastoma</t>
   </si>
   <si>
@@ -1559,6 +1553,12 @@
   </si>
   <si>
     <t>sequencing_protocol.paired_end</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.diseases.text</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.diseases.ontology</t>
   </si>
 </sst>
 </file>
@@ -2002,7 +2002,7 @@
     <col min="8" max="8" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2119,7 +2119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -2139,7 +2139,7 @@
     <col min="12" max="12" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="90" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>223</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>449</v>
       </c>
       <c r="J4" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K4" t="s">
         <v>454</v>
@@ -2271,19 +2271,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J6" t="s">
         <v>452</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -2311,7 +2311,7 @@
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>47</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2394,7 +2394,7 @@
         <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2410,7 +2410,7 @@
         <v>460</v>
       </c>
       <c r="D6" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H6" t="s">
         <v>456</v>
@@ -2478,7 +2478,7 @@
     <col min="47" max="47" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="180" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" ht="192" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>155</v>
       </c>
       <c r="AR4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="AS4" t="s">
         <v>160</v>
@@ -2929,7 +2929,7 @@
         <v>464</v>
       </c>
       <c r="AQ6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="AR6" t="s">
         <v>463</v>
@@ -2944,8 +2944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2983,7 +2983,7 @@
     <col min="34" max="35" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="360" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="380" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -3143,10 +3143,10 @@
         <v>189</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>470</v>
+        <v>508</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>471</v>
+        <v>509</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>62</v>
@@ -3255,10 +3255,10 @@
         <v>190</v>
       </c>
       <c r="R4" t="s">
-        <v>470</v>
+        <v>508</v>
       </c>
       <c r="S4" t="s">
-        <v>471</v>
+        <v>509</v>
       </c>
       <c r="T4" t="s">
         <v>191</v>
@@ -3334,16 +3334,16 @@
         <v>468</v>
       </c>
       <c r="I6" t="s">
+        <v>497</v>
+      </c>
+      <c r="J6" t="s">
+        <v>498</v>
+      </c>
+      <c r="K6" t="s">
         <v>499</v>
       </c>
-      <c r="J6" t="s">
-        <v>500</v>
-      </c>
-      <c r="K6" t="s">
-        <v>501</v>
-      </c>
       <c r="R6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="V6" t="s">
         <v>467</v>
@@ -3394,7 +3394,7 @@
     <col min="31" max="32" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="360" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="380" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -3508,10 +3508,10 @@
         <v>62</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>308</v>
@@ -3623,13 +3623,13 @@
         <v>231</v>
       </c>
       <c r="G4" t="s">
+        <v>502</v>
+      </c>
+      <c r="H4" t="s">
+        <v>503</v>
+      </c>
+      <c r="I4" t="s">
         <v>504</v>
-      </c>
-      <c r="H4" t="s">
-        <v>505</v>
-      </c>
-      <c r="I4" t="s">
-        <v>506</v>
       </c>
       <c r="J4" t="s">
         <v>232</v>
@@ -3717,10 +3717,10 @@
         <v>9606</v>
       </c>
       <c r="AE6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="AF6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -3749,7 +3749,7 @@
     <col min="11" max="11" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="270" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>281</v>
       </c>
@@ -3872,13 +3872,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B6" t="s">
         <v>469</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E6" t="s">
         <v>292</v>
@@ -3887,39 +3887,39 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="K6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B7" t="s">
         <v>469</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E7" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F7" s="5">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J7" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="K7" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -3953,7 +3953,7 @@
     <col min="14" max="14" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="165" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="176" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>223</v>
       </c>
@@ -4113,16 +4113,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>484</v>
+      </c>
+      <c r="B6" t="s">
+        <v>485</v>
+      </c>
+      <c r="G6" t="s">
         <v>486</v>
       </c>
-      <c r="B6" t="s">
+      <c r="H6" t="s">
         <v>487</v>
-      </c>
-      <c r="G6" t="s">
-        <v>488</v>
-      </c>
-      <c r="H6" t="s">
-        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -4153,7 +4153,7 @@
     <col min="10" max="11" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="105" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="112" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>223</v>
       </c>
@@ -4276,13 +4276,13 @@
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -4344,7 +4344,7 @@
     <col min="45" max="45" width="71.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="270" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>223</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>408</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="AB4" s="2" t="s">
         <v>412</v>
@@ -4813,27 +4813,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>472</v>
+      </c>
+      <c r="K6" t="s">
+        <v>473</v>
+      </c>
+      <c r="M6" t="s">
         <v>474</v>
       </c>
-      <c r="K6" t="s">
+      <c r="N6" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>493</v>
+      </c>
+      <c r="AB6" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="M6" t="s">
-        <v>476</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>490</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>495</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>477</v>
-      </c>
       <c r="AC6" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AD6" t="s">
         <v>418</v>

</xml_diff>

<commit_message>
Update int test spreadsheets with funder info.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/playground/cbeta_bundle_downloads/pancreas6decades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DAC51B-B0FF-D542-98F0-7535869276F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39EEDE9-9553-9744-ACA1-4F67B2D3EBA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="460" windowWidth="42320" windowHeight="25580" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8120" yWindow="460" windowWidth="31880" windowHeight="19820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -4356,7 +4356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -5817,7 +5817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update integration test spreadsheets to be valid.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39EEDE9-9553-9744-ACA1-4F67B2D3EBA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC687F8-B370-6048-A029-32CA7A39CD7D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8120" yWindow="460" windowWidth="31880" windowHeight="19820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,9 +346,6 @@
     <t xml:space="preserve"> For example: Biotechnology and Biological Sciences Research Council (BBSRC)</t>
   </si>
   <si>
-    <t>project.funders.funder_name</t>
-  </si>
-  <si>
     <t>BIOMATERIAL ID (Required)</t>
   </si>
   <si>
@@ -2219,6 +2216,9 @@
   </si>
   <si>
     <t>process.process_core.process_id</t>
+  </si>
+  <si>
+    <t>project.funders.organization</t>
   </si>
 </sst>
 </file>
@@ -2774,25 +2774,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>588</v>
+      </c>
+      <c r="B6" t="s">
+        <v>588</v>
+      </c>
+      <c r="C6" t="s">
+        <v>590</v>
+      </c>
+      <c r="D6" t="s">
         <v>589</v>
       </c>
-      <c r="B6" t="s">
-        <v>589</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
+        <v>726</v>
+      </c>
+      <c r="G6" t="s">
         <v>591</v>
       </c>
-      <c r="D6" t="s">
-        <v>590</v>
-      </c>
-      <c r="F6" t="s">
-        <v>727</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>592</v>
-      </c>
-      <c r="H6" t="s">
-        <v>593</v>
       </c>
     </row>
   </sheetData>
@@ -2818,60 +2818,60 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2885,13 +2885,13 @@
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>91</v>
@@ -2905,31 +2905,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>449</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2947,31 +2947,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B6" t="s">
+        <v>684</v>
+      </c>
+      <c r="C6" t="s">
         <v>685</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>679</v>
+      </c>
+      <c r="E6" t="s">
+        <v>680</v>
+      </c>
+      <c r="F6" t="s">
+        <v>681</v>
+      </c>
+      <c r="G6" t="s">
+        <v>688</v>
+      </c>
+      <c r="H6" t="s">
         <v>686</v>
       </c>
-      <c r="D6" t="s">
-        <v>680</v>
-      </c>
-      <c r="E6" t="s">
-        <v>681</v>
-      </c>
-      <c r="F6" t="s">
-        <v>682</v>
-      </c>
-      <c r="G6" t="s">
-        <v>689</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>687</v>
-      </c>
-      <c r="I6" t="s">
-        <v>688</v>
       </c>
     </row>
   </sheetData>
@@ -2998,78 +2998,78 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
@@ -3083,13 +3083,13 @@
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>91</v>
@@ -3101,51 +3101,51 @@
         <v>91</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>461</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3166,34 +3166,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>690</v>
+      </c>
+      <c r="B6" t="s">
         <v>691</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>692</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>679</v>
+      </c>
+      <c r="E6" t="s">
+        <v>680</v>
+      </c>
+      <c r="F6" t="s">
+        <v>681</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="J6" t="s">
         <v>693</v>
-      </c>
-      <c r="D6" t="s">
-        <v>680</v>
-      </c>
-      <c r="E6" t="s">
-        <v>681</v>
-      </c>
-      <c r="F6" t="s">
-        <v>682</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>695</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="J6" t="s">
-        <v>694</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3232,198 +3232,198 @@
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="68" x14ac:dyDescent="0.2">
@@ -3437,25 +3437,25 @@
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>91</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>91</v>
@@ -3467,7 +3467,7 @@
         <v>91</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>91</v>
@@ -3479,147 +3479,147 @@
         <v>91</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>485</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="W4" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>543</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="AC4" s="3" t="s">
-        <v>548</v>
-      </c>
       <c r="AD4" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3660,84 +3660,84 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>697</v>
+      </c>
+      <c r="B6" t="s">
+        <v>699</v>
+      </c>
+      <c r="C6" t="s">
         <v>698</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>679</v>
+      </c>
+      <c r="E6" t="s">
+        <v>680</v>
+      </c>
+      <c r="F6" t="s">
+        <v>681</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>700</v>
       </c>
-      <c r="C6" t="s">
-        <v>699</v>
-      </c>
-      <c r="D6" t="s">
-        <v>680</v>
-      </c>
-      <c r="E6" t="s">
-        <v>681</v>
-      </c>
-      <c r="F6" t="s">
-        <v>682</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>701</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>702</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>701</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>703</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>704</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>705</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>704</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>706</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
       <c r="T6" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="U6" t="s">
         <v>707</v>
-      </c>
-      <c r="U6" t="s">
-        <v>708</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" t="s">
+        <v>708</v>
+      </c>
+      <c r="X6" t="s">
         <v>709</v>
-      </c>
-      <c r="X6" t="s">
-        <v>710</v>
       </c>
       <c r="Y6">
         <v>20014279</v>
       </c>
       <c r="Z6" t="s">
+        <v>706</v>
+      </c>
+      <c r="AA6" t="s">
         <v>707</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>708</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="AD6" s="6" t="s">
+        <v>710</v>
+      </c>
+      <c r="AE6" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>712</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>713</v>
       </c>
     </row>
   </sheetData>
@@ -3767,90 +3767,90 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -3864,13 +3864,13 @@
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>91</v>
@@ -3882,10 +3882,10 @@
         <v>91</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>91</v>
@@ -3899,46 +3899,46 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>564</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>566</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3961,46 +3961,46 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B6" t="s">
+        <v>713</v>
+      </c>
+      <c r="C6" t="s">
         <v>714</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>679</v>
+      </c>
+      <c r="E6" t="s">
+        <v>680</v>
+      </c>
+      <c r="F6" t="s">
+        <v>681</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>715</v>
       </c>
-      <c r="D6" t="s">
-        <v>680</v>
-      </c>
-      <c r="E6" t="s">
-        <v>681</v>
-      </c>
-      <c r="F6" t="s">
-        <v>682</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>716</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="J6" t="s">
         <v>717</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>606</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="K6" t="s">
-        <v>607</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>719</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>720</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
   </sheetData>
@@ -4167,66 +4167,66 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D6" t="s">
+        <v>600</v>
+      </c>
+      <c r="E6" t="s">
         <v>601</v>
       </c>
-      <c r="E6" t="s">
-        <v>602</v>
-      </c>
       <c r="F6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G6" t="s">
+        <v>605</v>
+      </c>
+      <c r="H6" t="s">
         <v>606</v>
       </c>
-      <c r="H6" t="s">
-        <v>607</v>
-      </c>
       <c r="I6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="J6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C7" t="s">
+        <v>598</v>
+      </c>
+      <c r="D7" t="s">
         <v>599</v>
       </c>
-      <c r="D7" t="s">
-        <v>600</v>
-      </c>
       <c r="E7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F7" t="s">
+        <v>604</v>
+      </c>
+      <c r="G7" t="s">
         <v>605</v>
       </c>
-      <c r="G7" t="s">
-        <v>606</v>
-      </c>
       <c r="H7" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I7" t="s">
+        <v>609</v>
+      </c>
+      <c r="J7" t="s">
         <v>610</v>
-      </c>
-      <c r="J7" t="s">
-        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -4329,19 +4329,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>611</v>
+      </c>
+      <c r="B6" t="s">
         <v>612</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>613</v>
-      </c>
-      <c r="C6" t="s">
-        <v>614</v>
       </c>
       <c r="D6">
         <v>27565351</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
   </sheetData>
@@ -4357,7 +4357,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4398,7 +4398,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>96</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>104</v>
+        <v>728</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4418,13 +4418,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>615</v>
+      </c>
+      <c r="B6" t="s">
         <v>616</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>617</v>
-      </c>
-      <c r="C6" t="s">
-        <v>618</v>
       </c>
     </row>
   </sheetData>
@@ -4482,270 +4482,270 @@
   <sheetData>
     <row r="1" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:44" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:44" ht="85" x14ac:dyDescent="0.2">
@@ -4759,22 +4759,22 @@
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>91</v>
@@ -4795,13 +4795,13 @@
         <v>91</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>91</v>
@@ -4831,7 +4831,7 @@
         <v>91</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC3" s="2" t="s">
         <v>91</v>
@@ -4843,7 +4843,7 @@
         <v>91</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AG3" s="2" t="s">
         <v>91</v>
@@ -4855,7 +4855,7 @@
         <v>91</v>
       </c>
       <c r="AJ3" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>91</v>
@@ -4867,7 +4867,7 @@
         <v>91</v>
       </c>
       <c r="AN3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AO3" s="2" t="s">
         <v>91</v>
@@ -4879,141 +4879,141 @@
         <v>91</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5066,121 +5066,121 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>618</v>
+      </c>
+      <c r="B6" t="s">
         <v>619</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>620</v>
-      </c>
-      <c r="C6" t="s">
-        <v>621</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>621</v>
+      </c>
+      <c r="F6" t="s">
+        <v>624</v>
+      </c>
+      <c r="G6" t="s">
         <v>622</v>
       </c>
-      <c r="F6" t="s">
-        <v>625</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>623</v>
-      </c>
-      <c r="H6" t="s">
-        <v>624</v>
       </c>
       <c r="I6">
         <v>36.4</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>628</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="P6" t="s">
         <v>630</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>629</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
+        <v>630</v>
+      </c>
+      <c r="R6" t="s">
         <v>631</v>
       </c>
-      <c r="Q6" t="s">
-        <v>631</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="S6" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="U6" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="V6" t="s">
         <v>634</v>
       </c>
-      <c r="U6" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>635</v>
       </c>
-      <c r="W6" t="s">
-        <v>636</v>
-      </c>
       <c r="X6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Y6" t="s">
+        <v>720</v>
+      </c>
+      <c r="Z6" t="s">
         <v>721</v>
       </c>
-      <c r="Z6" t="s">
-        <v>722</v>
-      </c>
       <c r="AA6" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
+        <v>636</v>
+      </c>
+      <c r="AD6" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AE6" t="s">
         <v>638</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>639</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
+        <v>639</v>
+      </c>
+      <c r="AH6" t="s">
         <v>640</v>
       </c>
-      <c r="AH6" t="s">
-        <v>641</v>
-      </c>
       <c r="AI6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
+        <v>642</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="AM6" t="s">
         <v>643</v>
-      </c>
-      <c r="AL6" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -5192,7 +5192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK6"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="Y1" workbookViewId="0">
       <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
@@ -5221,216 +5221,216 @@
   <sheetData>
     <row r="1" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:37" ht="68" x14ac:dyDescent="0.2">
@@ -5444,19 +5444,19 @@
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>91</v>
@@ -5495,34 +5495,34 @@
         <v>91</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>91</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE3" s="2" t="s">
         <v>91</v>
@@ -5534,124 +5534,124 @@
         <v>91</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AK3" s="2"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>240</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5697,115 +5697,115 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>645</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>646</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>621</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="G6" t="s">
         <v>622</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>625</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>623</v>
       </c>
-      <c r="H6" t="s">
-        <v>624</v>
-      </c>
       <c r="I6" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>630</v>
-      </c>
       <c r="K6" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="L6" t="s">
+        <v>646</v>
+      </c>
+      <c r="M6" t="s">
         <v>647</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
+        <v>646</v>
+      </c>
+      <c r="O6" t="s">
+        <v>722</v>
+      </c>
+      <c r="P6" t="s">
+        <v>723</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>722</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="U6" t="s">
         <v>648</v>
       </c>
-      <c r="N6" t="s">
-        <v>647</v>
-      </c>
-      <c r="O6" t="s">
-        <v>723</v>
-      </c>
-      <c r="P6" t="s">
-        <v>724</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>723</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>722</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>649</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>650</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>651</v>
-      </c>
-      <c r="X6" t="s">
-        <v>652</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
+        <v>652</v>
+      </c>
+      <c r="AA6" t="s">
         <v>653</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>654</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="AG6" s="3" t="s">
-        <v>639</v>
-      </c>
       <c r="AH6" t="s">
+        <v>654</v>
+      </c>
+      <c r="AI6" t="s">
         <v>655</v>
       </c>
-      <c r="AI6" t="s">
-        <v>656</v>
-      </c>
       <c r="AJ6" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -5841,168 +5841,168 @@
   <sheetData>
     <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="68" x14ac:dyDescent="0.2">
@@ -6016,25 +6016,25 @@
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>91</v>
@@ -6046,16 +6046,16 @@
         <v>91</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>91</v>
@@ -6076,108 +6076,108 @@
         <v>91</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>327</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6216,73 +6216,73 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>658</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>659</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>621</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="G6" t="s">
         <v>622</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>625</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>623</v>
       </c>
-      <c r="H6" t="s">
-        <v>624</v>
-      </c>
       <c r="I6" t="s">
+        <v>660</v>
+      </c>
+      <c r="J6" t="s">
         <v>661</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>662</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>663</v>
       </c>
-      <c r="L6" t="s">
-        <v>664</v>
-      </c>
       <c r="M6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
+        <v>664</v>
+      </c>
+      <c r="P6" t="s">
         <v>665</v>
-      </c>
-      <c r="P6" t="s">
-        <v>666</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
       <c r="R6" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="S6" s="3" t="s">
-        <v>630</v>
-      </c>
       <c r="T6" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="U6" t="s">
+        <v>666</v>
+      </c>
+      <c r="V6" t="s">
         <v>667</v>
       </c>
-      <c r="V6" t="s">
-        <v>668</v>
-      </c>
       <c r="W6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6291,19 +6291,19 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AA6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="AC6" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="AD6" s="3" t="s">
         <v>690</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>691</v>
       </c>
     </row>
   </sheetData>
@@ -6327,54 +6327,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -6382,63 +6382,63 @@
         <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>396</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6458,13 +6458,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6473,16 +6473,16 @@
         <v>75</v>
       </c>
       <c r="G6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -6490,13 +6490,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>670</v>
+      </c>
+      <c r="B7" t="s">
         <v>671</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" s="3" t="s">
         <v>672</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>673</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6505,16 +6505,16 @@
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -6557,60 +6557,60 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -6624,13 +6624,13 @@
         <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>91</v>
@@ -6644,31 +6644,31 @@
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6686,31 +6686,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>676</v>
+      </c>
+      <c r="B6" t="s">
         <v>677</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>678</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>679</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>680</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>681</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>682</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>683</v>
       </c>
-      <c r="H6" t="s">
-        <v>684</v>
-      </c>
       <c r="I6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated SS2 integration test spreadsheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25936172-C896-D144-81F8-13A8C0B44BD9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73F88FA-6A50-3E41-8660-F9D63096468F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1165,18 +1165,12 @@
     <t>cell_suspension.plate_based_sequencing.well_id</t>
   </si>
   <si>
-    <t>CELL QUALITY</t>
-  </si>
-  <si>
     <t>Note on how good cell looks if imaged in well before sequencing.</t>
   </si>
   <si>
     <t xml:space="preserve"> For example: Should be one of: 'OK', 'control, 2-cell well', 'control, empty well', or 'low quality cell'.</t>
   </si>
   <si>
-    <t>cell_suspension.plate_based_sequencing.cell_quality</t>
-  </si>
-  <si>
     <t>FILE NAME (Required)</t>
   </si>
   <si>
@@ -2219,6 +2213,12 @@
   </si>
   <si>
     <t>cell_suspension.estimated_cell_count</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.well_quality</t>
+  </si>
+  <si>
+    <t>WELL QUALITY</t>
   </si>
 </sst>
 </file>
@@ -2748,16 +2748,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>725</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>726</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2774,25 +2774,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>581</v>
+      </c>
+      <c r="B6" t="s">
+        <v>581</v>
+      </c>
+      <c r="C6" t="s">
         <v>583</v>
       </c>
-      <c r="B6" t="s">
-        <v>583</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>582</v>
+      </c>
+      <c r="F6" t="s">
+        <v>719</v>
+      </c>
+      <c r="G6" t="s">
+        <v>584</v>
+      </c>
+      <c r="H6" t="s">
         <v>585</v>
-      </c>
-      <c r="D6" t="s">
-        <v>584</v>
-      </c>
-      <c r="F6" t="s">
-        <v>721</v>
-      </c>
-      <c r="G6" t="s">
-        <v>586</v>
-      </c>
-      <c r="H6" t="s">
-        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -2818,54 +2818,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>420</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -2885,13 +2885,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -2905,31 +2905,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>447</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2947,31 +2947,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B6" t="s">
+        <v>677</v>
+      </c>
+      <c r="C6" t="s">
+        <v>678</v>
+      </c>
+      <c r="D6" t="s">
+        <v>672</v>
+      </c>
+      <c r="E6" t="s">
+        <v>673</v>
+      </c>
+      <c r="F6" t="s">
+        <v>674</v>
+      </c>
+      <c r="G6" t="s">
+        <v>681</v>
+      </c>
+      <c r="H6" t="s">
         <v>679</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I6" t="s">
         <v>680</v>
-      </c>
-      <c r="D6" t="s">
-        <v>674</v>
-      </c>
-      <c r="E6" t="s">
-        <v>675</v>
-      </c>
-      <c r="F6" t="s">
-        <v>676</v>
-      </c>
-      <c r="G6" t="s">
-        <v>683</v>
-      </c>
-      <c r="H6" t="s">
-        <v>681</v>
-      </c>
-      <c r="I6" t="s">
-        <v>682</v>
       </c>
     </row>
   </sheetData>
@@ -2998,63 +2998,63 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>462</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>420</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -3063,13 +3063,13 @@
         <v>139</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
@@ -3083,13 +3083,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -3101,51 +3101,51 @@
         <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>461</v>
-      </c>
       <c r="J4" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3166,34 +3166,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>683</v>
+      </c>
+      <c r="B6" t="s">
+        <v>684</v>
+      </c>
+      <c r="C6" t="s">
         <v>685</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>672</v>
+      </c>
+      <c r="E6" t="s">
+        <v>673</v>
+      </c>
+      <c r="F6" t="s">
+        <v>674</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="J6" t="s">
         <v>686</v>
-      </c>
-      <c r="C6" t="s">
-        <v>687</v>
-      </c>
-      <c r="D6" t="s">
-        <v>674</v>
-      </c>
-      <c r="E6" t="s">
-        <v>675</v>
-      </c>
-      <c r="F6" t="s">
-        <v>676</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>689</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>690</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="J6" t="s">
-        <v>688</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3232,135 +3232,135 @@
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>502</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>513</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>420</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>136</v>
@@ -3369,10 +3369,10 @@
         <v>139</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>136</v>
@@ -3381,49 +3381,49 @@
         <v>139</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="68" x14ac:dyDescent="0.2">
@@ -3437,25 +3437,25 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>87</v>
@@ -3467,7 +3467,7 @@
         <v>87</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>87</v>
@@ -3479,147 +3479,147 @@
         <v>87</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>479</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>501</v>
-      </c>
       <c r="N4" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>512</v>
-      </c>
       <c r="R4" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="W4" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="Y4" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="AB4" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>542</v>
-      </c>
       <c r="AD4" s="3" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3660,84 +3660,84 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>690</v>
+      </c>
+      <c r="B6" t="s">
         <v>692</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>691</v>
+      </c>
+      <c r="D6" t="s">
+        <v>672</v>
+      </c>
+      <c r="E6" t="s">
+        <v>673</v>
+      </c>
+      <c r="F6" t="s">
+        <v>674</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="C6" t="s">
+      <c r="M6" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="D6" t="s">
-        <v>674</v>
-      </c>
-      <c r="E6" t="s">
-        <v>675</v>
-      </c>
-      <c r="F6" t="s">
-        <v>676</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>695</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>698</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>699</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>698</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>700</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="U6" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="X6" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="Y6">
         <v>20014279</v>
       </c>
       <c r="Z6" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="AA6" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
+        <v>701</v>
+      </c>
+      <c r="AD6" s="6" t="s">
         <v>703</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AE6" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>705</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>706</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -3767,69 +3767,69 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>568</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>420</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -3838,13 +3838,13 @@
         <v>139</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>136</v>
@@ -3864,13 +3864,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -3882,10 +3882,10 @@
         <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>87</v>
@@ -3899,46 +3899,46 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>560</v>
-      </c>
       <c r="G4" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>567</v>
-      </c>
       <c r="J4" s="3" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>580</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3961,46 +3961,46 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B6" t="s">
+        <v>706</v>
+      </c>
+      <c r="C6" t="s">
+        <v>707</v>
+      </c>
+      <c r="D6" t="s">
+        <v>672</v>
+      </c>
+      <c r="E6" t="s">
+        <v>673</v>
+      </c>
+      <c r="F6" t="s">
+        <v>674</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" s="3" t="s">
         <v>709</v>
       </c>
-      <c r="D6" t="s">
-        <v>674</v>
-      </c>
-      <c r="E6" t="s">
-        <v>675</v>
-      </c>
-      <c r="F6" t="s">
-        <v>676</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="J6" t="s">
         <v>710</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="K6" t="s">
+        <v>599</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>710</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="M6" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="K6" t="s">
-        <v>601</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>713</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>714</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
   </sheetData>
@@ -4167,66 +4167,66 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>586</v>
+      </c>
+      <c r="B6" t="s">
         <v>588</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>590</v>
       </c>
-      <c r="C6" t="s">
-        <v>592</v>
-      </c>
       <c r="D6" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E6" t="s">
+        <v>594</v>
+      </c>
+      <c r="F6" t="s">
         <v>596</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>598</v>
       </c>
-      <c r="G6" t="s">
-        <v>600</v>
-      </c>
       <c r="H6" t="s">
+        <v>599</v>
+      </c>
+      <c r="I6" t="s">
         <v>601</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>603</v>
-      </c>
-      <c r="J6" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>587</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" t="s">
         <v>591</v>
       </c>
-      <c r="C7" t="s">
-        <v>593</v>
-      </c>
       <c r="D7" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E7" t="s">
+        <v>595</v>
+      </c>
+      <c r="F7" t="s">
         <v>597</v>
       </c>
-      <c r="F7" t="s">
-        <v>599</v>
-      </c>
       <c r="G7" t="s">
+        <v>598</v>
+      </c>
+      <c r="H7" t="s">
         <v>600</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>602</v>
       </c>
-      <c r="I7" t="s">
-        <v>604</v>
-      </c>
       <c r="J7" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
   </sheetData>
@@ -4329,19 +4329,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>604</v>
+      </c>
+      <c r="B6" t="s">
+        <v>605</v>
+      </c>
+      <c r="C6" t="s">
         <v>606</v>
-      </c>
-      <c r="B6" t="s">
-        <v>607</v>
-      </c>
-      <c r="C6" t="s">
-        <v>608</v>
       </c>
       <c r="D6">
         <v>27565351</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -4406,7 +4406,7 @@
         <v>96</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4418,13 +4418,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B6" t="s">
+        <v>609</v>
+      </c>
+      <c r="C6" t="s">
         <v>610</v>
-      </c>
-      <c r="B6" t="s">
-        <v>611</v>
-      </c>
-      <c r="C6" t="s">
-        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -5066,121 +5066,121 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>611</v>
+      </c>
+      <c r="B6" t="s">
+        <v>612</v>
+      </c>
+      <c r="C6" t="s">
         <v>613</v>
-      </c>
-      <c r="B6" t="s">
-        <v>614</v>
-      </c>
-      <c r="C6" t="s">
-        <v>615</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>614</v>
+      </c>
+      <c r="F6" t="s">
+        <v>617</v>
+      </c>
+      <c r="G6" t="s">
+        <v>615</v>
+      </c>
+      <c r="H6" t="s">
         <v>616</v>
-      </c>
-      <c r="F6" t="s">
-        <v>619</v>
-      </c>
-      <c r="G6" t="s">
-        <v>617</v>
-      </c>
-      <c r="H6" t="s">
-        <v>618</v>
       </c>
       <c r="I6">
         <v>36.4</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="P6" t="s">
         <v>623</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="Q6" t="s">
+        <v>623</v>
+      </c>
+      <c r="R6" t="s">
         <v>624</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="S6" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="U6" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="R6" t="s">
-        <v>626</v>
-      </c>
-      <c r="S6" s="3" t="s">
+      <c r="V6" t="s">
         <v>627</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="W6" t="s">
         <v>628</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="X6" t="s">
         <v>627</v>
       </c>
-      <c r="V6" t="s">
-        <v>629</v>
-      </c>
-      <c r="W6" t="s">
-        <v>630</v>
-      </c>
-      <c r="X6" t="s">
-        <v>629</v>
-      </c>
       <c r="Y6" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="Z6" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="AA6" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
+        <v>629</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="AE6" t="s">
         <v>631</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>633</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="AH6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="AI6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="AL6" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="AM6" t="s">
         <v>636</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -5651,7 +5651,7 @@
         <v>102</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5697,115 +5697,115 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>614</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="G6" t="s">
+        <v>615</v>
+      </c>
+      <c r="H6" t="s">
         <v>616</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>619</v>
-      </c>
-      <c r="G6" t="s">
-        <v>617</v>
-      </c>
-      <c r="H6" t="s">
-        <v>618</v>
-      </c>
       <c r="I6" s="3" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="L6" t="s">
+        <v>639</v>
+      </c>
+      <c r="M6" t="s">
+        <v>640</v>
+      </c>
+      <c r="N6" t="s">
+        <v>639</v>
+      </c>
+      <c r="O6" t="s">
+        <v>715</v>
+      </c>
+      <c r="P6" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>715</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="U6" t="s">
         <v>641</v>
       </c>
-      <c r="M6" t="s">
+      <c r="V6" t="s">
         <v>642</v>
       </c>
-      <c r="N6" t="s">
-        <v>641</v>
-      </c>
-      <c r="O6" t="s">
-        <v>717</v>
-      </c>
-      <c r="P6" t="s">
-        <v>718</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>717</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>715</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>715</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>643</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>644</v>
-      </c>
-      <c r="W6" t="s">
-        <v>645</v>
-      </c>
-      <c r="X6" t="s">
-        <v>646</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="AA6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="AF6" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="AG6" s="3" t="s">
-        <v>633</v>
-      </c>
       <c r="AH6" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="AI6" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -5818,7 +5818,7 @@
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5919,7 +5919,7 @@
         <v>373</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>377</v>
+        <v>728</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
@@ -6002,7 +6002,7 @@
         <v>374</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="68" x14ac:dyDescent="0.2">
@@ -6085,7 +6085,7 @@
         <v>375</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -6159,7 +6159,7 @@
         <v>365</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="Y4" s="3" t="s">
         <v>372</v>
@@ -6168,16 +6168,16 @@
         <v>376</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>380</v>
+        <v>727</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>228</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6216,73 +6216,73 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>651</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>652</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>653</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>614</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="G6" t="s">
+        <v>615</v>
+      </c>
+      <c r="H6" t="s">
         <v>616</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>619</v>
-      </c>
-      <c r="G6" t="s">
-        <v>617</v>
-      </c>
-      <c r="H6" t="s">
-        <v>618</v>
-      </c>
       <c r="I6" t="s">
+        <v>653</v>
+      </c>
+      <c r="J6" t="s">
+        <v>654</v>
+      </c>
+      <c r="K6" t="s">
         <v>655</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>656</v>
       </c>
-      <c r="K6" t="s">
-        <v>657</v>
-      </c>
-      <c r="L6" t="s">
-        <v>658</v>
-      </c>
       <c r="M6" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="P6" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="U6" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="V6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="W6" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6291,19 +6291,19 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="AA6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -6327,54 +6327,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>383</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>384</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -6382,63 +6382,63 @@
         <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>390</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>315</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6458,13 +6458,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>662</v>
+      </c>
+      <c r="B6" t="s">
         <v>664</v>
       </c>
-      <c r="B6" t="s">
-        <v>666</v>
-      </c>
       <c r="D6" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6473,16 +6473,16 @@
         <v>75</v>
       </c>
       <c r="G6" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -6490,13 +6490,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>663</v>
+      </c>
+      <c r="B7" t="s">
+        <v>664</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>665</v>
-      </c>
-      <c r="B7" t="s">
-        <v>666</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>667</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6505,16 +6505,16 @@
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -6557,54 +6557,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>420</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -6624,13 +6624,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -6644,31 +6644,31 @@
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>435</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6686,31 +6686,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>669</v>
+      </c>
+      <c r="B6" t="s">
+        <v>670</v>
+      </c>
+      <c r="C6" t="s">
         <v>671</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>672</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>673</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>674</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>675</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>676</v>
       </c>
-      <c r="G6" t="s">
-        <v>677</v>
-      </c>
-      <c r="H6" t="s">
-        <v>678</v>
-      </c>
       <c r="I6" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated SS2 inteagration test spreadsheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA390A4-A9EE-F04F-918C-9A5631828550}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2978F1-FF0A-1643-B10B-2296E97A8927}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1141,30 +1141,18 @@
     <t>Enter 1 for well-based assays. For example: 2100</t>
   </si>
   <si>
-    <t>WELL PLATE ID (Required)</t>
-  </si>
-  <si>
     <t>An ID for the plate that the well is located on.</t>
   </si>
   <si>
     <t xml:space="preserve"> For example: 2217</t>
   </si>
   <si>
-    <t>cell_suspension.plate_based_sequencing.plate_id</t>
-  </si>
-  <si>
-    <t>WELL ID</t>
-  </si>
-  <si>
     <t>An ID or name for the well. Should be unique for the plate.</t>
   </si>
   <si>
     <t xml:space="preserve"> For example: A1</t>
   </si>
   <si>
-    <t>cell_suspension.plate_based_sequencing.well_id</t>
-  </si>
-  <si>
     <t>CELL QUALITY</t>
   </si>
   <si>
@@ -2219,6 +2207,18 @@
   </si>
   <si>
     <t>sequencing_protocol.method.ontology_label</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.plate_label</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.well_label</t>
+  </si>
+  <si>
+    <t>PLATE LABEL (Required)</t>
+  </si>
+  <si>
+    <t>WELL LABEL</t>
   </si>
 </sst>
 </file>
@@ -2748,16 +2748,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2774,25 +2774,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>566</v>
+      </c>
+      <c r="B6" t="s">
+        <v>566</v>
+      </c>
+      <c r="C6" t="s">
+        <v>568</v>
+      </c>
+      <c r="D6" t="s">
+        <v>567</v>
+      </c>
+      <c r="F6" t="s">
+        <v>704</v>
+      </c>
+      <c r="G6" t="s">
+        <v>569</v>
+      </c>
+      <c r="H6" t="s">
         <v>570</v>
-      </c>
-      <c r="B6" t="s">
-        <v>570</v>
-      </c>
-      <c r="C6" t="s">
-        <v>572</v>
-      </c>
-      <c r="D6" t="s">
-        <v>571</v>
-      </c>
-      <c r="F6" t="s">
-        <v>708</v>
-      </c>
-      <c r="G6" t="s">
-        <v>573</v>
-      </c>
-      <c r="H6" t="s">
-        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -2818,54 +2818,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>426</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>431</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -2885,13 +2885,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>428</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -2905,31 +2905,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>439</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2947,31 +2947,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="B6" t="s">
+        <v>662</v>
+      </c>
+      <c r="C6" t="s">
+        <v>663</v>
+      </c>
+      <c r="D6" t="s">
+        <v>657</v>
+      </c>
+      <c r="E6" t="s">
+        <v>658</v>
+      </c>
+      <c r="F6" t="s">
+        <v>659</v>
+      </c>
+      <c r="G6" t="s">
         <v>666</v>
       </c>
-      <c r="C6" t="s">
-        <v>667</v>
-      </c>
-      <c r="D6" t="s">
-        <v>661</v>
-      </c>
-      <c r="E6" t="s">
-        <v>662</v>
-      </c>
-      <c r="F6" t="s">
-        <v>663</v>
-      </c>
-      <c r="G6" t="s">
-        <v>670</v>
-      </c>
       <c r="H6" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="I6" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
   </sheetData>
@@ -2998,63 +2998,63 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>426</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>431</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -3063,13 +3063,13 @@
         <v>139</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>460</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
@@ -3083,14 +3083,14 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>428</v>
-      </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
       </c>
@@ -3101,51 +3101,51 @@
         <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>462</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3166,34 +3166,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>668</v>
+      </c>
+      <c r="B6" t="s">
+        <v>669</v>
+      </c>
+      <c r="C6" t="s">
+        <v>670</v>
+      </c>
+      <c r="D6" t="s">
+        <v>657</v>
+      </c>
+      <c r="E6" t="s">
+        <v>658</v>
+      </c>
+      <c r="F6" t="s">
+        <v>659</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="B6" t="s">
+      <c r="H6" s="3" t="s">
         <v>673</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I6" s="3" t="s">
         <v>674</v>
       </c>
-      <c r="D6" t="s">
-        <v>661</v>
-      </c>
-      <c r="E6" t="s">
-        <v>662</v>
-      </c>
-      <c r="F6" t="s">
-        <v>663</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>678</v>
-      </c>
       <c r="J6" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3232,135 +3232,135 @@
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>426</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>477</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>488</v>
-      </c>
       <c r="L1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="X1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="AD1" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>427</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>478</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>485</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>489</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>136</v>
@@ -3369,10 +3369,10 @@
         <v>139</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>500</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>136</v>
@@ -3381,49 +3381,49 @@
         <v>139</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>524</v>
-      </c>
       <c r="X2" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>524</v>
-      </c>
       <c r="AD2" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="68" x14ac:dyDescent="0.2">
@@ -3437,26 +3437,26 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>428</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>486</v>
-      </c>
       <c r="K3" s="2" t="s">
         <v>87</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>87</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>87</v>
@@ -3479,147 +3479,147 @@
         <v>87</v>
       </c>
       <c r="R3" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="W3" s="2" t="s">
-        <v>525</v>
-      </c>
       <c r="X3" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="AC3" s="2" t="s">
-        <v>525</v>
-      </c>
       <c r="AD3" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>539</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>476</v>
-      </c>
       <c r="H4" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>487</v>
-      </c>
       <c r="K4" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>498</v>
-      </c>
       <c r="O4" s="3" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA4" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="Z4" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>540</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3660,84 +3660,84 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>675</v>
+      </c>
+      <c r="B6" t="s">
+        <v>677</v>
+      </c>
+      <c r="C6" t="s">
+        <v>676</v>
+      </c>
+      <c r="D6" t="s">
+        <v>657</v>
+      </c>
+      <c r="E6" t="s">
+        <v>658</v>
+      </c>
+      <c r="F6" t="s">
+        <v>659</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="B6" t="s">
+      <c r="M6" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="C6" t="s">
-        <v>680</v>
-      </c>
-      <c r="D6" t="s">
-        <v>661</v>
-      </c>
-      <c r="E6" t="s">
-        <v>662</v>
-      </c>
-      <c r="F6" t="s">
-        <v>663</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>683</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>686</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>687</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="U6" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="X6" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="Y6">
         <v>20014279</v>
       </c>
       <c r="Z6" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="AA6" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
+        <v>686</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>688</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>690</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>692</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>693</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -3749,7 +3749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -3767,69 +3767,69 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>426</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>566</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>427</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -3838,13 +3838,13 @@
         <v>139</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>567</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>136</v>
@@ -3864,14 +3864,14 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>428</v>
-      </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
       </c>
@@ -3882,10 +3882,10 @@
         <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>564</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>87</v>
@@ -3899,46 +3899,46 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>565</v>
-      </c>
       <c r="L4" s="3" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3961,46 +3961,46 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="B6" t="s">
+        <v>691</v>
+      </c>
+      <c r="C6" t="s">
+        <v>692</v>
+      </c>
+      <c r="D6" t="s">
+        <v>657</v>
+      </c>
+      <c r="E6" t="s">
+        <v>658</v>
+      </c>
+      <c r="F6" t="s">
+        <v>659</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="J6" t="s">
         <v>695</v>
       </c>
-      <c r="C6" t="s">
+      <c r="K6" t="s">
+        <v>584</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="D6" t="s">
-        <v>661</v>
-      </c>
-      <c r="E6" t="s">
-        <v>662</v>
-      </c>
-      <c r="F6" t="s">
-        <v>663</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>698</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="J6" t="s">
-        <v>699</v>
-      </c>
-      <c r="K6" t="s">
-        <v>588</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>700</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>701</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -4167,66 +4167,66 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>571</v>
+      </c>
+      <c r="B6" t="s">
+        <v>573</v>
+      </c>
+      <c r="C6" t="s">
         <v>575</v>
       </c>
-      <c r="B6" t="s">
-        <v>577</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>578</v>
+      </c>
+      <c r="E6" t="s">
         <v>579</v>
       </c>
-      <c r="D6" t="s">
-        <v>582</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>581</v>
+      </c>
+      <c r="G6" t="s">
         <v>583</v>
       </c>
-      <c r="F6" t="s">
-        <v>585</v>
-      </c>
-      <c r="G6" t="s">
-        <v>587</v>
-      </c>
       <c r="H6" t="s">
+        <v>584</v>
+      </c>
+      <c r="I6" t="s">
+        <v>586</v>
+      </c>
+      <c r="J6" t="s">
         <v>588</v>
-      </c>
-      <c r="I6" t="s">
-        <v>590</v>
-      </c>
-      <c r="J6" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>572</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="C7" t="s">
         <v>576</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>577</v>
+      </c>
+      <c r="E7" t="s">
         <v>580</v>
       </c>
-      <c r="D7" t="s">
-        <v>581</v>
-      </c>
-      <c r="E7" t="s">
-        <v>584</v>
-      </c>
       <c r="F7" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="G7" t="s">
+        <v>583</v>
+      </c>
+      <c r="H7" t="s">
+        <v>585</v>
+      </c>
+      <c r="I7" t="s">
         <v>587</v>
       </c>
-      <c r="H7" t="s">
-        <v>589</v>
-      </c>
-      <c r="I7" t="s">
-        <v>591</v>
-      </c>
       <c r="J7" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
   </sheetData>
@@ -4329,19 +4329,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B6" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C6" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D6">
         <v>27565351</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>
@@ -4406,7 +4406,7 @@
         <v>96</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4418,13 +4418,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B6" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C6" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -5066,121 +5066,121 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B6" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C6" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="F6" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="G6" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H6" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="I6">
         <v>36.4</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>607</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="P6" t="s">
         <v>608</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="Q6" t="s">
+        <v>608</v>
+      </c>
+      <c r="R6" t="s">
         <v>609</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="S6" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="U6" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="P6" t="s">
+      <c r="V6" t="s">
         <v>612</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="W6" t="s">
+        <v>613</v>
+      </c>
+      <c r="X6" t="s">
         <v>612</v>
       </c>
-      <c r="R6" t="s">
-        <v>613</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>614</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>615</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>614</v>
-      </c>
-      <c r="V6" t="s">
-        <v>616</v>
-      </c>
-      <c r="W6" t="s">
-        <v>617</v>
-      </c>
-      <c r="X6" t="s">
-        <v>616</v>
-      </c>
       <c r="Y6" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="Z6" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="AA6" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="AE6" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="AH6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="AI6" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="AL6" s="3" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="AM6" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>
@@ -5651,7 +5651,7 @@
         <v>102</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5697,115 +5697,115 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="G6" t="s">
+        <v>600</v>
+      </c>
+      <c r="H6" t="s">
+        <v>601</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="G6" t="s">
-        <v>604</v>
-      </c>
-      <c r="H6" t="s">
-        <v>605</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>610</v>
-      </c>
       <c r="J6" s="3" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="L6" t="s">
+        <v>624</v>
+      </c>
+      <c r="M6" t="s">
+        <v>625</v>
+      </c>
+      <c r="N6" t="s">
+        <v>624</v>
+      </c>
+      <c r="O6" t="s">
+        <v>700</v>
+      </c>
+      <c r="P6" t="s">
+        <v>701</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>700</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="U6" t="s">
+        <v>626</v>
+      </c>
+      <c r="V6" t="s">
+        <v>627</v>
+      </c>
+      <c r="W6" t="s">
         <v>628</v>
       </c>
-      <c r="M6" t="s">
+      <c r="X6" t="s">
         <v>629</v>
-      </c>
-      <c r="N6" t="s">
-        <v>628</v>
-      </c>
-      <c r="O6" t="s">
-        <v>704</v>
-      </c>
-      <c r="P6" t="s">
-        <v>705</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>704</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>702</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>703</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>702</v>
-      </c>
-      <c r="U6" t="s">
-        <v>630</v>
-      </c>
-      <c r="V6" t="s">
-        <v>631</v>
-      </c>
-      <c r="W6" t="s">
-        <v>632</v>
-      </c>
-      <c r="X6" t="s">
-        <v>633</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="AA6" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="AG6" s="3" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="AH6" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="AI6" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -5817,8 +5817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5913,13 +5913,13 @@
         <v>366</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>369</v>
+        <v>727</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>373</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
@@ -5996,13 +5996,13 @@
         <v>367</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Z2" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="68" x14ac:dyDescent="0.2">
@@ -6079,13 +6079,13 @@
         <v>368</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Z3" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -6159,25 +6159,25 @@
         <v>365</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>372</v>
+        <v>725</v>
       </c>
       <c r="Z4" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="AA4" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>380</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>228</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6216,73 +6216,73 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="G6" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H6" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="I6" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="J6" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="K6" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="L6" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="M6" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="P6" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="U6" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="V6" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="W6" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6291,19 +6291,19 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="AA6" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -6327,54 +6327,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>403</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>404</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -6382,63 +6382,63 @@
         <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>402</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>315</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6458,13 +6458,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="B6" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="D6" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6473,16 +6473,16 @@
         <v>75</v>
       </c>
       <c r="G6" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -6490,13 +6490,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="B7" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6505,16 +6505,16 @@
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -6557,54 +6557,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>430</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>431</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -6624,13 +6624,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>428</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -6644,31 +6644,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>429</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6686,31 +6686,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>654</v>
+      </c>
+      <c r="B6" t="s">
+        <v>655</v>
+      </c>
+      <c r="C6" t="s">
+        <v>656</v>
+      </c>
+      <c r="D6" t="s">
+        <v>657</v>
+      </c>
+      <c r="E6" t="s">
         <v>658</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>659</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>660</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H6" t="s">
         <v>661</v>
       </c>
-      <c r="E6" t="s">
-        <v>662</v>
-      </c>
-      <c r="F6" t="s">
-        <v>663</v>
-      </c>
-      <c r="G6" t="s">
-        <v>664</v>
-      </c>
-      <c r="H6" t="s">
-        <v>665</v>
-      </c>
       <c r="I6" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated SS2 integration test sheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sehsan/Devel/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD8229A-FB38-AC46-93B6-11FB5541D581}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34640" yWindow="460" windowWidth="31120" windowHeight="19180" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="10900" yWindow="460" windowWidth="31120" windowHeight="19180" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
     <sheet name="Library preparation protocol" sheetId="13" r:id="rId12"/>
     <sheet name="Sequencing protocol" sheetId="14" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1157,9 +1158,6 @@
     <t xml:space="preserve"> For example: 2217</t>
   </si>
   <si>
-    <t>cell_suspension.plate_based_sequencing.plate_id</t>
-  </si>
-  <si>
     <t>WELL ID</t>
   </si>
   <si>
@@ -1169,9 +1167,6 @@
     <t xml:space="preserve"> For example: A1</t>
   </si>
   <si>
-    <t>cell_suspension.plate_based_sequencing.well_id</t>
-  </si>
-  <si>
     <t>Note on how good cell looks if imaged in well before sequencing.</t>
   </si>
   <si>
@@ -2226,12 +2221,18 @@
   </si>
   <si>
     <t>LIBRARY_PREPARATION_PROTOCOL.LIBRARY_CONSTRUCTION_METHOD.TEXT (Required)</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.well_label</t>
+  </si>
+  <si>
+    <t>cell_suspension.plate_based_sequencing.plate_label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2615,7 +2616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2655,7 +2656,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2681,7 +2682,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2721,16 +2722,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>716</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>717</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>718</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2747,25 +2748,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>573</v>
+      </c>
+      <c r="B6" t="s">
+        <v>573</v>
+      </c>
+      <c r="C6" t="s">
         <v>575</v>
       </c>
-      <c r="B6" t="s">
-        <v>575</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>574</v>
+      </c>
+      <c r="F6" t="s">
+        <v>711</v>
+      </c>
+      <c r="G6" t="s">
+        <v>576</v>
+      </c>
+      <c r="H6" t="s">
         <v>577</v>
-      </c>
-      <c r="D6" t="s">
-        <v>576</v>
-      </c>
-      <c r="F6" t="s">
-        <v>713</v>
-      </c>
-      <c r="G6" t="s">
-        <v>578</v>
-      </c>
-      <c r="H6" t="s">
-        <v>579</v>
       </c>
     </row>
   </sheetData>
@@ -2774,7 +2775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2791,54 +2792,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -2847,7 +2848,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -2858,13 +2859,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -2878,31 +2879,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>445</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2920,31 +2921,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B6" t="s">
+        <v>669</v>
+      </c>
+      <c r="C6" t="s">
+        <v>670</v>
+      </c>
+      <c r="D6" t="s">
+        <v>664</v>
+      </c>
+      <c r="E6" t="s">
+        <v>665</v>
+      </c>
+      <c r="F6" t="s">
+        <v>666</v>
+      </c>
+      <c r="G6" t="s">
+        <v>673</v>
+      </c>
+      <c r="H6" t="s">
         <v>671</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I6" t="s">
         <v>672</v>
-      </c>
-      <c r="D6" t="s">
-        <v>666</v>
-      </c>
-      <c r="E6" t="s">
-        <v>667</v>
-      </c>
-      <c r="F6" t="s">
-        <v>668</v>
-      </c>
-      <c r="G6" t="s">
-        <v>675</v>
-      </c>
-      <c r="H6" t="s">
-        <v>673</v>
-      </c>
-      <c r="I6" t="s">
-        <v>674</v>
       </c>
     </row>
   </sheetData>
@@ -2953,7 +2954,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2971,63 +2972,63 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>460</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -3036,16 +3037,16 @@
         <v>139</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -3056,13 +3057,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -3074,51 +3075,51 @@
         <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>459</v>
-      </c>
       <c r="J4" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3139,34 +3140,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>675</v>
+      </c>
+      <c r="B6" t="s">
+        <v>676</v>
+      </c>
+      <c r="C6" t="s">
         <v>677</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>664</v>
+      </c>
+      <c r="E6" t="s">
+        <v>665</v>
+      </c>
+      <c r="F6" t="s">
+        <v>666</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="J6" t="s">
         <v>678</v>
-      </c>
-      <c r="C6" t="s">
-        <v>679</v>
-      </c>
-      <c r="D6" t="s">
-        <v>666</v>
-      </c>
-      <c r="E6" t="s">
-        <v>667</v>
-      </c>
-      <c r="F6" t="s">
-        <v>668</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="J6" t="s">
-        <v>680</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3181,10 +3182,10 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
@@ -3205,135 +3206,135 @@
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>500</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="64" x14ac:dyDescent="0.2">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>136</v>
@@ -3342,10 +3343,10 @@
         <v>139</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>136</v>
@@ -3354,52 +3355,52 @@
         <v>139</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="64" x14ac:dyDescent="0.2">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -3410,25 +3411,25 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>87</v>
@@ -3440,7 +3441,7 @@
         <v>87</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>87</v>
@@ -3452,147 +3453,147 @@
         <v>87</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>477</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>499</v>
-      </c>
       <c r="N4" s="3" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="W4" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="Y4" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="AB4" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>534</v>
-      </c>
       <c r="AD4" s="3" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3633,84 +3634,84 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>682</v>
+      </c>
+      <c r="B6" t="s">
         <v>684</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>683</v>
+      </c>
+      <c r="D6" t="s">
+        <v>664</v>
+      </c>
+      <c r="E6" t="s">
+        <v>665</v>
+      </c>
+      <c r="F6" t="s">
+        <v>666</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>686</v>
       </c>
-      <c r="C6" t="s">
+      <c r="M6" s="3" t="s">
         <v>685</v>
       </c>
-      <c r="D6" t="s">
-        <v>666</v>
-      </c>
-      <c r="E6" t="s">
-        <v>667</v>
-      </c>
-      <c r="F6" t="s">
-        <v>668</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>688</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>689</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>690</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>690</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>692</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="U6" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="X6" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="Y6">
         <v>20014279</v>
       </c>
       <c r="Z6" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="AA6" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
+        <v>693</v>
+      </c>
+      <c r="AD6" s="6" t="s">
         <v>695</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AE6" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>697</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>698</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>699</v>
       </c>
     </row>
   </sheetData>
@@ -3719,7 +3720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3740,69 +3741,69 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>560</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -3811,13 +3812,13 @@
         <v>139</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>136</v>
@@ -3826,7 +3827,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -3837,13 +3838,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -3855,10 +3856,10 @@
         <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>87</v>
@@ -3872,46 +3873,46 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>552</v>
-      </c>
       <c r="G4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>559</v>
-      </c>
       <c r="J4" s="3" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>572</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3934,46 +3935,46 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B6" t="s">
+        <v>698</v>
+      </c>
+      <c r="C6" t="s">
+        <v>699</v>
+      </c>
+      <c r="D6" t="s">
+        <v>664</v>
+      </c>
+      <c r="E6" t="s">
+        <v>665</v>
+      </c>
+      <c r="F6" t="s">
+        <v>666</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>700</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" s="3" t="s">
         <v>701</v>
       </c>
-      <c r="D6" t="s">
-        <v>666</v>
-      </c>
-      <c r="E6" t="s">
-        <v>667</v>
-      </c>
-      <c r="F6" t="s">
-        <v>668</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="J6" t="s">
         <v>702</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="K6" t="s">
+        <v>591</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>703</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>702</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="M6" s="3" t="s">
         <v>704</v>
       </c>
-      <c r="K6" t="s">
-        <v>593</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>705</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>706</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
   </sheetData>
@@ -3982,7 +3983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4028,7 +4029,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -4060,7 +4061,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -4140,78 +4141,78 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B6" t="s">
         <v>580</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>582</v>
       </c>
-      <c r="C6" t="s">
-        <v>584</v>
-      </c>
       <c r="D6" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E6" t="s">
+        <v>586</v>
+      </c>
+      <c r="F6" t="s">
         <v>588</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>590</v>
       </c>
-      <c r="G6" t="s">
-        <v>592</v>
-      </c>
       <c r="H6" t="s">
+        <v>591</v>
+      </c>
+      <c r="I6" t="s">
         <v>593</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>595</v>
-      </c>
-      <c r="J6" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>579</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" t="s">
         <v>583</v>
       </c>
-      <c r="C7" t="s">
-        <v>585</v>
-      </c>
       <c r="D7" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E7" t="s">
+        <v>587</v>
+      </c>
+      <c r="F7" t="s">
         <v>589</v>
       </c>
-      <c r="F7" t="s">
-        <v>591</v>
-      </c>
       <c r="G7" t="s">
+        <v>590</v>
+      </c>
+      <c r="H7" t="s">
         <v>592</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>594</v>
       </c>
-      <c r="I7" t="s">
-        <v>596</v>
-      </c>
       <c r="J7" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4240,7 +4241,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
@@ -4257,7 +4258,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>71</v>
       </c>
@@ -4302,31 +4303,31 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B6" t="s">
+        <v>597</v>
+      </c>
+      <c r="C6" t="s">
         <v>598</v>
-      </c>
-      <c r="B6" t="s">
-        <v>599</v>
-      </c>
-      <c r="C6" t="s">
-        <v>600</v>
       </c>
       <c r="D6">
         <v>27565351</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4349,7 +4350,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -4360,7 +4361,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>91</v>
       </c>
@@ -4379,7 +4380,7 @@
         <v>96</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4391,13 +4392,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>600</v>
+      </c>
+      <c r="B6" t="s">
+        <v>601</v>
+      </c>
+      <c r="C6" t="s">
         <v>602</v>
-      </c>
-      <c r="B6" t="s">
-        <v>603</v>
-      </c>
-      <c r="C6" t="s">
-        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -4406,7 +4407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
@@ -4587,7 +4588,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:44" ht="112" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>101</v>
       </c>
@@ -4721,7 +4722,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:44" ht="80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -5039,121 +5040,121 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>603</v>
+      </c>
+      <c r="B6" t="s">
+        <v>604</v>
+      </c>
+      <c r="C6" t="s">
         <v>605</v>
-      </c>
-      <c r="B6" t="s">
-        <v>606</v>
-      </c>
-      <c r="C6" t="s">
-        <v>607</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>606</v>
+      </c>
+      <c r="F6" t="s">
+        <v>609</v>
+      </c>
+      <c r="G6" t="s">
+        <v>607</v>
+      </c>
+      <c r="H6" t="s">
         <v>608</v>
-      </c>
-      <c r="F6" t="s">
-        <v>611</v>
-      </c>
-      <c r="G6" t="s">
-        <v>609</v>
-      </c>
-      <c r="H6" t="s">
-        <v>610</v>
       </c>
       <c r="I6">
         <v>36.4</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="P6" t="s">
         <v>615</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="Q6" t="s">
+        <v>615</v>
+      </c>
+      <c r="R6" t="s">
         <v>616</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>615</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="S6" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="U6" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="R6" t="s">
-        <v>618</v>
-      </c>
-      <c r="S6" s="3" t="s">
+      <c r="V6" t="s">
         <v>619</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="W6" t="s">
         <v>620</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="X6" t="s">
         <v>619</v>
       </c>
-      <c r="V6" t="s">
-        <v>621</v>
-      </c>
-      <c r="W6" t="s">
-        <v>622</v>
-      </c>
-      <c r="X6" t="s">
-        <v>621</v>
-      </c>
       <c r="Y6" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="Z6" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="AA6" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
+        <v>621</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="AE6" t="s">
         <v>623</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>625</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="AH6" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="AI6" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="AL6" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="AM6" t="s">
         <v>628</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -5162,7 +5163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK6"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
@@ -5299,7 +5300,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="112" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>101</v>
       </c>
@@ -5406,7 +5407,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -5624,7 +5625,7 @@
         <v>102</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5670,115 +5671,115 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>606</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="G6" t="s">
+        <v>607</v>
+      </c>
+      <c r="H6" t="s">
         <v>608</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="G6" t="s">
-        <v>609</v>
-      </c>
-      <c r="H6" t="s">
-        <v>610</v>
-      </c>
       <c r="I6" s="3" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L6" t="s">
+        <v>631</v>
+      </c>
+      <c r="M6" t="s">
+        <v>632</v>
+      </c>
+      <c r="N6" t="s">
+        <v>631</v>
+      </c>
+      <c r="O6" t="s">
+        <v>707</v>
+      </c>
+      <c r="P6" t="s">
+        <v>708</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>707</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="U6" t="s">
         <v>633</v>
       </c>
-      <c r="M6" t="s">
+      <c r="V6" t="s">
         <v>634</v>
       </c>
-      <c r="N6" t="s">
-        <v>633</v>
-      </c>
-      <c r="O6" t="s">
-        <v>709</v>
-      </c>
-      <c r="P6" t="s">
-        <v>710</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>709</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>707</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>707</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>635</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>636</v>
-      </c>
-      <c r="W6" t="s">
-        <v>637</v>
-      </c>
-      <c r="X6" t="s">
-        <v>638</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="AA6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="AF6" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="AG6" s="3" t="s">
-        <v>625</v>
-      </c>
       <c r="AH6" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="AI6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
   </sheetData>
@@ -5787,11 +5788,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5889,13 +5890,13 @@
         <v>369</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" ht="112" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>101</v>
       </c>
@@ -5972,13 +5973,13 @@
         <v>370</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" ht="64" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -6055,10 +6056,10 @@
         <v>371</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -6132,25 +6133,25 @@
         <v>365</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>372</v>
+        <v>728</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>376</v>
+        <v>727</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>228</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6189,73 +6190,73 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>643</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>645</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>606</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="G6" t="s">
+        <v>607</v>
+      </c>
+      <c r="H6" t="s">
         <v>608</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="G6" t="s">
-        <v>609</v>
-      </c>
-      <c r="H6" t="s">
-        <v>610</v>
-      </c>
       <c r="I6" t="s">
+        <v>645</v>
+      </c>
+      <c r="J6" t="s">
+        <v>646</v>
+      </c>
+      <c r="K6" t="s">
         <v>647</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>648</v>
       </c>
-      <c r="K6" t="s">
-        <v>649</v>
-      </c>
-      <c r="L6" t="s">
-        <v>650</v>
-      </c>
       <c r="M6" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="P6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="V6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="W6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6264,19 +6265,19 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="AA6" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>
@@ -6285,7 +6286,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6300,118 +6301,118 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>405</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="80" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="112" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>388</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>315</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6431,13 +6432,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>654</v>
+      </c>
+      <c r="B6" t="s">
         <v>656</v>
       </c>
-      <c r="B6" t="s">
-        <v>658</v>
-      </c>
       <c r="D6" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6446,16 +6447,16 @@
         <v>75</v>
       </c>
       <c r="G6" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -6463,13 +6464,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>655</v>
+      </c>
+      <c r="B7" t="s">
+        <v>656</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>657</v>
-      </c>
-      <c r="B7" t="s">
-        <v>658</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>659</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6478,16 +6479,16 @@
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -6513,7 +6514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6530,54 +6531,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -6586,7 +6587,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -6597,13 +6598,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -6617,31 +6618,31 @@
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>433</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6659,31 +6660,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>661</v>
+      </c>
+      <c r="B6" t="s">
+        <v>662</v>
+      </c>
+      <c r="C6" t="s">
         <v>663</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>664</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>665</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>666</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>667</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>668</v>
       </c>
-      <c r="G6" t="s">
-        <v>669</v>
-      </c>
-      <c r="H6" t="s">
-        <v>670</v>
-      </c>
       <c r="I6" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated integration test spreadsheets with content_description fields. Fixes #1033.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548DE58D-B9E0-1543-A992-B3ECD329EC32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4816C85-A6F8-D742-8355-CB701BAE1BE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="746">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -2227,6 +2227,57 @@
   </si>
   <si>
     <t>sequence_file.insdc_run_accessions</t>
+  </si>
+  <si>
+    <t>General description of the contents of the file.</t>
+  </si>
+  <si>
+    <t>An ontology term identifier in the form prefix:accession.</t>
+  </si>
+  <si>
+    <t>The preferred label for the ontology term referred to in the ontology field. This may differ from the user-supplied value in the text field.</t>
+  </si>
+  <si>
+    <t>sequence_file.file_core.content_description.text</t>
+  </si>
+  <si>
+    <t>sequence_file.file_core.content_description.ontology</t>
+  </si>
+  <si>
+    <t>sequence_file.file_core.content_description.ontology_label</t>
+  </si>
+  <si>
+    <t>For example: DNA sequence (raw); Sequence alignment</t>
+  </si>
+  <si>
+    <t>For example: DATA:3497; DATA:0863</t>
+  </si>
+  <si>
+    <t>DNA sequence (raw)</t>
+  </si>
+  <si>
+    <t>data:3497</t>
+  </si>
+  <si>
+    <t>CONTENT DESCRIPTION</t>
+  </si>
+  <si>
+    <t>CONTENT DESCRIPTION ONTOLOGY</t>
+  </si>
+  <si>
+    <t>CONTENT DESCRIPTION ONTOLOGY LABEL</t>
+  </si>
+  <si>
+    <t>SOURCE CELL SUSPENSION ID</t>
+  </si>
+  <si>
+    <t>LIBRARY PREPARATION PROTOCOL ID</t>
+  </si>
+  <si>
+    <t>SEQUENCING PROTOCOL ID</t>
+  </si>
+  <si>
+    <t>PROCESS ID</t>
   </si>
 </sst>
 </file>
@@ -2299,7 +2350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2312,6 +2363,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6287,135 +6341,190 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="25.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="9" width="25.6640625" customWidth="1"/>
+    <col min="10" max="10" width="24" style="3" customWidth="1"/>
+    <col min="11" max="11" width="31.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="37.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="33.83203125" customWidth="1"/>
+    <col min="14" max="14" width="24.1640625" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>357</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J3" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>364</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>728</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>302</v>
-      </c>
       <c r="J4" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -6429,84 +6538,106 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>618</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="C6" t="s">
         <v>620</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>623</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>75</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>624</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>738</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="L6">
+      <c r="O6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>619</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="C7" t="s">
         <v>620</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>75</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>624</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>738</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="L7">
+      <c r="O7">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed ontology and ontology label for DNA Sequence on integration spreadsheets.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/HumanCellAtlas/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4816C85-A6F8-D742-8355-CB701BAE1BE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA10366-53A2-0846-8D7B-D13EC2C7D468}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2253,12 +2253,6 @@
     <t>For example: DATA:3497; DATA:0863</t>
   </si>
   <si>
-    <t>DNA sequence (raw)</t>
-  </si>
-  <si>
-    <t>data:3497</t>
-  </si>
-  <si>
     <t>CONTENT DESCRIPTION</t>
   </si>
   <si>
@@ -2278,13 +2272,19 @@
   </si>
   <si>
     <t>PROCESS ID</t>
+  </si>
+  <si>
+    <t>DNA sequence</t>
+  </si>
+  <si>
+    <t>data:3494</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2321,6 +2321,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2363,9 +2370,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6344,7 +6349,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="J6" sqref="J6:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6365,7 +6370,7 @@
         <v>357</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>359</v>
@@ -6389,22 +6394,22 @@
         <v>381</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>744</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
@@ -6543,7 +6548,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>618</v>
       </c>
@@ -6566,13 +6571,13 @@
         <v>624</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>737</v>
+        <v>744</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>738</v>
+        <v>745</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>737</v>
+        <v>744</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>646</v>
@@ -6584,7 +6589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>619</v>
       </c>
@@ -6607,13 +6612,13 @@
         <v>624</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>737</v>
+        <v>744</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>738</v>
+        <v>745</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>737</v>
+        <v>744</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>646</v>

</xml_diff>

<commit_message>
reverse project/study in SS2 spreadsheet
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshadbolt/Desktop/git_repos/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49D0D1F-57D3-DA43-A3E3-CC44F2FDBCBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8A4D07-8996-B849-A9BF-62484E050A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46840" yWindow="5560" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32480" yWindow="2580" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -2682,7 +2682,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2822,7 +2822,7 @@
         <v>536</v>
       </c>
       <c r="E6" t="s">
-        <v>539</v>
+        <v>744</v>
       </c>
       <c r="F6" t="s">
         <v>673</v>
@@ -2831,7 +2831,7 @@
         <v>538</v>
       </c>
       <c r="H6" t="s">
-        <v>744</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Official HCA publication field to SS2 spreadsheet
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshadbolt/Desktop/git_repos/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karoly/dev/hca/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8A4D07-8996-B849-A9BF-62484E050A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4148E954-09B0-3D4B-8052-E2B49931F488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32480" yWindow="2580" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-5940" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="752">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -2281,6 +2281,21 @@
   </si>
   <si>
     <t>Enter accession if project has been archived. Accession can be from the DDBJ, NCBI, or EMBL-EBI and must start with PRJD, PRJN, or PRJE, respectively. For example: PRJNA000000</t>
+  </si>
+  <si>
+    <t>OFFICIAL HCA PUBLICATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> For example: Yes/No</t>
+  </si>
+  <si>
+    <t>A boolean field to defined if this project is the offical HCA publication.</t>
+  </si>
+  <si>
+    <t>project.publications.official_hca_publication</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -2681,7 +2696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -4278,18 +4293,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="25.6640625" customWidth="1"/>
+    <col min="1" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -4305,8 +4322,11 @@
       <c r="E1" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -4322,8 +4342,11 @@
       <c r="E2" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F2" s="2" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
@@ -4339,8 +4362,11 @@
       <c r="E3" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
@@ -4356,8 +4382,11 @@
       <c r="E4" s="3" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="3" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4365,8 +4394,9 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>558</v>
       </c>
@@ -4381,6 +4411,9 @@
       </c>
       <c r="E6" s="4" t="s">
         <v>561</v>
+      </c>
+      <c r="F6" t="s">
+        <v>751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove wrong accessions from the SS2 sample spreadsheet
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karoly/dev/hca/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4148E954-09B0-3D4B-8052-E2B49931F488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CE5370-08FB-6648-8E18-DB9E7B74BFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-5940" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-5940" windowWidth="51200" windowHeight="28340" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="751">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -1747,9 +1747,6 @@
   </si>
   <si>
     <t>DRB1 0401 protective allele</t>
-  </si>
-  <si>
-    <t>SAMN00000000</t>
   </si>
   <si>
     <t>SRS0000000</t>
@@ -2773,7 +2770,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
@@ -2782,7 +2779,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2799,16 +2796,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>676</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>677</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>678</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2837,10 +2834,10 @@
         <v>536</v>
       </c>
       <c r="E6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G6" t="s">
         <v>538</v>
@@ -2977,13 +2974,13 @@
         <v>412</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>698</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3001,31 +2998,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B6" t="s">
+        <v>630</v>
+      </c>
+      <c r="C6" t="s">
         <v>631</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>625</v>
+      </c>
+      <c r="E6" t="s">
+        <v>626</v>
+      </c>
+      <c r="F6" t="s">
+        <v>627</v>
+      </c>
+      <c r="G6" t="s">
+        <v>634</v>
+      </c>
+      <c r="H6" t="s">
         <v>632</v>
       </c>
-      <c r="D6" t="s">
-        <v>626</v>
-      </c>
-      <c r="E6" t="s">
-        <v>627</v>
-      </c>
-      <c r="F6" t="s">
-        <v>628</v>
-      </c>
-      <c r="G6" t="s">
-        <v>635</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>633</v>
-      </c>
-      <c r="I6" t="s">
-        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -3184,22 +3181,22 @@
         <v>421</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>716</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>717</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>718</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>428</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>719</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3220,34 +3217,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B6" t="s">
         <v>637</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>638</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>625</v>
+      </c>
+      <c r="E6" t="s">
+        <v>626</v>
+      </c>
+      <c r="F6" t="s">
+        <v>627</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="J6" t="s">
         <v>639</v>
-      </c>
-      <c r="D6" t="s">
-        <v>626</v>
-      </c>
-      <c r="E6" t="s">
-        <v>627</v>
-      </c>
-      <c r="F6" t="s">
-        <v>628</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="J6" t="s">
-        <v>640</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3328,13 +3325,13 @@
         <v>463</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>685</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>686</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>468</v>
@@ -3622,13 +3619,13 @@
         <v>466</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>471</v>
@@ -3714,84 +3711,84 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>643</v>
+      </c>
+      <c r="B6" t="s">
+        <v>645</v>
+      </c>
+      <c r="C6" t="s">
         <v>644</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>625</v>
+      </c>
+      <c r="E6" t="s">
+        <v>626</v>
+      </c>
+      <c r="F6" t="s">
+        <v>627</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="C6" t="s">
-        <v>645</v>
-      </c>
-      <c r="D6" t="s">
-        <v>626</v>
-      </c>
-      <c r="E6" t="s">
-        <v>627</v>
-      </c>
-      <c r="F6" t="s">
-        <v>628</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>650</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>651</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>652</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
       <c r="T6" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="U6" t="s">
         <v>653</v>
-      </c>
-      <c r="U6" t="s">
-        <v>654</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" t="s">
+        <v>654</v>
+      </c>
+      <c r="X6" t="s">
         <v>655</v>
-      </c>
-      <c r="X6" t="s">
-        <v>656</v>
       </c>
       <c r="Y6">
         <v>20014279</v>
       </c>
       <c r="Z6" t="s">
+        <v>652</v>
+      </c>
+      <c r="AA6" t="s">
         <v>653</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>654</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="AD6" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="AE6" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>658</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>659</v>
       </c>
     </row>
   </sheetData>
@@ -3986,13 +3983,13 @@
         <v>530</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>700</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>701</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4015,46 +4012,46 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B6" t="s">
+        <v>659</v>
+      </c>
+      <c r="C6" t="s">
         <v>660</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>625</v>
+      </c>
+      <c r="E6" t="s">
+        <v>626</v>
+      </c>
+      <c r="F6" t="s">
+        <v>627</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>661</v>
       </c>
-      <c r="D6" t="s">
-        <v>626</v>
-      </c>
-      <c r="E6" t="s">
-        <v>627</v>
-      </c>
-      <c r="F6" t="s">
-        <v>628</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="J6" t="s">
         <v>663</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="J6" t="s">
-        <v>664</v>
       </c>
       <c r="K6" t="s">
         <v>553</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>666</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
   </sheetData>
@@ -4175,7 +4172,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
@@ -4199,7 +4196,7 @@
         <v>57</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>64</v>
@@ -4295,7 +4292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -4323,7 +4320,7 @@
         <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4343,7 +4340,7 @@
         <v>81</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4363,7 +4360,7 @@
         <v>82</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4371,7 +4368,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>75</v>
@@ -4380,10 +4377,10 @@
         <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4413,7 +4410,7 @@
         <v>561</v>
       </c>
       <c r="F6" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
   </sheetData>
@@ -4478,7 +4475,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4509,7 +4506,7 @@
   <dimension ref="A1:AR6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="G4:H4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4974,10 +4971,10 @@
         <v>113</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>710</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>711</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>123</v>
@@ -5153,106 +5150,103 @@
         <v>568</v>
       </c>
       <c r="F6" t="s">
-        <v>571</v>
-      </c>
-      <c r="G6" t="s">
+        <v>570</v>
+      </c>
+      <c r="H6" t="s">
         <v>569</v>
-      </c>
-      <c r="H6" t="s">
-        <v>570</v>
       </c>
       <c r="I6">
         <v>36.4</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="P6" t="s">
         <v>576</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
+        <v>576</v>
+      </c>
+      <c r="R6" t="s">
         <v>577</v>
       </c>
-      <c r="Q6" t="s">
-        <v>577</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="S6" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="U6" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="V6" t="s">
         <v>580</v>
       </c>
-      <c r="U6" s="3" t="s">
-        <v>579</v>
-      </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>581</v>
       </c>
-      <c r="W6" t="s">
-        <v>582</v>
-      </c>
       <c r="X6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="Y6" t="s">
+        <v>666</v>
+      </c>
+      <c r="Z6" t="s">
         <v>667</v>
       </c>
-      <c r="Z6" t="s">
-        <v>668</v>
-      </c>
       <c r="AA6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
+        <v>582</v>
+      </c>
+      <c r="AD6" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AE6" t="s">
         <v>584</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>585</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
+        <v>585</v>
+      </c>
+      <c r="AH6" t="s">
         <v>586</v>
       </c>
-      <c r="AH6" t="s">
-        <v>587</v>
-      </c>
       <c r="AI6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
+        <v>588</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="AM6" t="s">
         <v>589</v>
-      </c>
-      <c r="AL6" s="3" t="s">
-        <v>588</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -5265,7 +5259,7 @@
   <dimension ref="A1:AK6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5633,10 +5627,10 @@
         <v>225</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>227</v>
@@ -5657,13 +5651,13 @@
         <v>238</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>689</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>690</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>691</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>244</v>
@@ -5681,7 +5675,7 @@
         <v>255</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>262</v>
@@ -5693,7 +5687,7 @@
         <v>270</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>277</v>
@@ -5769,13 +5763,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>592</v>
       </c>
       <c r="D6">
         <v>9606</v>
@@ -5784,100 +5778,97 @@
         <v>568</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="G6" t="s">
+        <v>570</v>
+      </c>
+      <c r="H6" t="s">
         <v>569</v>
       </c>
-      <c r="H6" t="s">
-        <v>570</v>
-      </c>
       <c r="I6" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>576</v>
-      </c>
       <c r="K6" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L6" t="s">
+        <v>592</v>
+      </c>
+      <c r="M6" t="s">
         <v>593</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
+        <v>592</v>
+      </c>
+      <c r="O6" t="s">
+        <v>668</v>
+      </c>
+      <c r="P6" t="s">
+        <v>669</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>668</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="U6" t="s">
         <v>594</v>
       </c>
-      <c r="N6" t="s">
-        <v>593</v>
-      </c>
-      <c r="O6" t="s">
-        <v>669</v>
-      </c>
-      <c r="P6" t="s">
-        <v>670</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>669</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>595</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>596</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>597</v>
-      </c>
-      <c r="X6" t="s">
-        <v>598</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
+        <v>598</v>
+      </c>
+      <c r="AA6" t="s">
         <v>599</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>600</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="AG6" s="3" t="s">
-        <v>585</v>
-      </c>
       <c r="AH6" t="s">
+        <v>600</v>
+      </c>
+      <c r="AI6" t="s">
         <v>601</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>602</v>
       </c>
       <c r="AJ6" s="3" t="s">
         <v>565</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -5889,8 +5880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5985,13 +5976,13 @@
         <v>346</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>706</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
@@ -6180,10 +6171,10 @@
         <v>305</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>714</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>715</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>309</v>
@@ -6222,25 +6213,25 @@
         <v>341</v>
       </c>
       <c r="U4" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="V4" s="3" t="s">
         <v>721</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>722</v>
       </c>
-      <c r="W4" s="3" t="s">
-        <v>723</v>
-      </c>
       <c r="X4" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="AA4" s="3" t="s">
         <v>680</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>703</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>704</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>681</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>220</v>
@@ -6288,13 +6279,13 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>604</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>605</v>
       </c>
       <c r="D6">
         <v>9606</v>
@@ -6303,58 +6294,55 @@
         <v>568</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="G6" t="s">
+        <v>570</v>
+      </c>
+      <c r="H6" t="s">
         <v>569</v>
       </c>
-      <c r="H6" t="s">
-        <v>570</v>
-      </c>
       <c r="I6" t="s">
+        <v>606</v>
+      </c>
+      <c r="J6" t="s">
         <v>607</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>608</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>609</v>
       </c>
-      <c r="L6" t="s">
-        <v>610</v>
-      </c>
       <c r="M6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
+        <v>610</v>
+      </c>
+      <c r="P6" t="s">
         <v>611</v>
-      </c>
-      <c r="P6" t="s">
-        <v>612</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
       <c r="R6" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="S6" s="3" t="s">
-        <v>576</v>
-      </c>
       <c r="T6" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="U6" t="s">
+        <v>612</v>
+      </c>
+      <c r="V6" t="s">
         <v>613</v>
       </c>
-      <c r="V6" t="s">
-        <v>614</v>
-      </c>
       <c r="W6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6363,19 +6351,19 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AA6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AC6" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="AD6" s="3" t="s">
         <v>636</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -6409,7 +6397,7 @@
         <v>355</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>357</v>
@@ -6433,22 +6421,22 @@
         <v>379</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>737</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>740</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
@@ -6477,13 +6465,13 @@
         <v>380</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>728</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="119" x14ac:dyDescent="0.2">
@@ -6512,13 +6500,13 @@
         <v>381</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>734</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -6529,7 +6517,7 @@
         <v>300</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>363</v>
@@ -6544,19 +6532,19 @@
         <v>375</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>382</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>731</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>732</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>435</v>
@@ -6565,7 +6553,7 @@
         <v>510</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6589,16 +6577,16 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C6" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -6607,22 +6595,22 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="J6" s="8" t="s">
+        <v>741</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>742</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>743</v>
-      </c>
       <c r="L6" s="8" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -6630,16 +6618,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>616</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="C7" t="s">
         <v>617</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>603</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E7" s="3" t="s">
         <v>618</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>619</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -6648,22 +6636,22 @@
         <v>75</v>
       </c>
       <c r="H7" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="J7" s="8" t="s">
+        <v>741</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>742</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>743</v>
-      </c>
       <c r="L7" s="8" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -6811,13 +6799,13 @@
         <v>402</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>695</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6835,31 +6823,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B6" t="s">
         <v>623</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>624</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>625</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>626</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>627</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>628</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>629</v>
       </c>
-      <c r="H6" t="s">
-        <v>630</v>
-      </c>
       <c r="I6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed donor ontology to use hsapdv
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshadbolt/Desktop/git_repos/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/HumanCellAtlas/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8A4D07-8996-B849-A9BF-62484E050A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE353635-E11F-4845-A5CA-43552F11C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32480" yWindow="2580" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26700" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1785,12 +1785,6 @@
     <t>UO:0000036</t>
   </si>
   <si>
-    <t>adult</t>
-  </si>
-  <si>
-    <t>EFO:0001272</t>
-  </si>
-  <si>
     <t>days</t>
   </si>
   <si>
@@ -2281,6 +2275,12 @@
   </si>
   <si>
     <t>Enter accession if project has been archived. Accession can be from the DDBJ, NCBI, or EMBL-EBI and must start with PRJD, PRJN, or PRJE, respectively. For example: PRJNA000000</t>
+  </si>
+  <si>
+    <t>human adult stage</t>
+  </si>
+  <si>
+    <t>HsapDv:0000087</t>
   </si>
 </sst>
 </file>
@@ -2681,7 +2681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2758,7 +2758,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
@@ -2767,7 +2767,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2784,16 +2784,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>676</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>677</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2822,10 +2822,10 @@
         <v>536</v>
       </c>
       <c r="E6" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F6" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="G6" t="s">
         <v>538</v>
@@ -2962,13 +2962,13 @@
         <v>412</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>697</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>698</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2986,31 +2986,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B6" t="s">
+        <v>629</v>
+      </c>
+      <c r="C6" t="s">
+        <v>630</v>
+      </c>
+      <c r="D6" t="s">
+        <v>624</v>
+      </c>
+      <c r="E6" t="s">
+        <v>625</v>
+      </c>
+      <c r="F6" t="s">
+        <v>626</v>
+      </c>
+      <c r="G6" t="s">
+        <v>633</v>
+      </c>
+      <c r="H6" t="s">
         <v>631</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I6" t="s">
         <v>632</v>
-      </c>
-      <c r="D6" t="s">
-        <v>626</v>
-      </c>
-      <c r="E6" t="s">
-        <v>627</v>
-      </c>
-      <c r="F6" t="s">
-        <v>628</v>
-      </c>
-      <c r="G6" t="s">
-        <v>635</v>
-      </c>
-      <c r="H6" t="s">
-        <v>633</v>
-      </c>
-      <c r="I6" t="s">
-        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -3169,22 +3169,22 @@
         <v>421</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>716</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>717</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>718</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>428</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3205,34 +3205,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>635</v>
+      </c>
+      <c r="B6" t="s">
+        <v>636</v>
+      </c>
+      <c r="C6" t="s">
         <v>637</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>624</v>
+      </c>
+      <c r="E6" t="s">
+        <v>625</v>
+      </c>
+      <c r="F6" t="s">
+        <v>626</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="J6" t="s">
         <v>638</v>
-      </c>
-      <c r="C6" t="s">
-        <v>639</v>
-      </c>
-      <c r="D6" t="s">
-        <v>626</v>
-      </c>
-      <c r="E6" t="s">
-        <v>627</v>
-      </c>
-      <c r="F6" t="s">
-        <v>628</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="J6" t="s">
-        <v>640</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3313,13 +3313,13 @@
         <v>463</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>468</v>
@@ -3607,13 +3607,13 @@
         <v>466</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>471</v>
@@ -3699,84 +3699,84 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>642</v>
+      </c>
+      <c r="B6" t="s">
         <v>644</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>643</v>
+      </c>
+      <c r="D6" t="s">
+        <v>624</v>
+      </c>
+      <c r="E6" t="s">
+        <v>625</v>
+      </c>
+      <c r="F6" t="s">
+        <v>626</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="C6" t="s">
+      <c r="M6" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="D6" t="s">
-        <v>626</v>
-      </c>
-      <c r="E6" t="s">
-        <v>627</v>
-      </c>
-      <c r="F6" t="s">
-        <v>628</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>650</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>651</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>652</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="U6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="X6" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="Y6">
         <v>20014279</v>
       </c>
       <c r="Z6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="AA6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
+        <v>653</v>
+      </c>
+      <c r="AD6" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AE6" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>657</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>658</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>659</v>
       </c>
     </row>
   </sheetData>
@@ -3971,13 +3971,13 @@
         <v>530</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>700</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>701</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4000,46 +4000,46 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B6" t="s">
+        <v>658</v>
+      </c>
+      <c r="C6" t="s">
+        <v>659</v>
+      </c>
+      <c r="D6" t="s">
+        <v>624</v>
+      </c>
+      <c r="E6" t="s">
+        <v>625</v>
+      </c>
+      <c r="F6" t="s">
+        <v>626</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>660</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" s="3" t="s">
         <v>661</v>
       </c>
-      <c r="D6" t="s">
-        <v>626</v>
-      </c>
-      <c r="E6" t="s">
-        <v>627</v>
-      </c>
-      <c r="F6" t="s">
-        <v>628</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="J6" t="s">
         <v>662</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="J6" t="s">
-        <v>664</v>
       </c>
       <c r="K6" t="s">
         <v>553</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
   </sheetData>
@@ -4160,7 +4160,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
@@ -4184,7 +4184,7 @@
         <v>57</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>64</v>
@@ -4345,7 +4345,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>75</v>
@@ -4354,7 +4354,7 @@
         <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4445,7 +4445,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4475,8 +4475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="G4:H4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4941,10 +4941,10 @@
         <v>113</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>123</v>
@@ -5168,58 +5168,58 @@
         <v>579</v>
       </c>
       <c r="V6" t="s">
-        <v>581</v>
+        <v>745</v>
       </c>
       <c r="W6" t="s">
-        <v>582</v>
-      </c>
-      <c r="X6" t="s">
-        <v>581</v>
+        <v>746</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>745</v>
       </c>
       <c r="Y6" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="Z6" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="AA6" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
+        <v>581</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="AE6" t="s">
         <v>583</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>585</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="AH6" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="AI6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="AL6" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="AM6" t="s">
         <v>588</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -5600,10 +5600,10 @@
         <v>225</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>227</v>
@@ -5624,13 +5624,13 @@
         <v>238</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>689</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>690</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>691</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>244</v>
@@ -5648,7 +5648,7 @@
         <v>255</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>262</v>
@@ -5660,7 +5660,7 @@
         <v>270</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>277</v>
@@ -5736,13 +5736,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D6">
         <v>9606</v>
@@ -5769,82 +5769,82 @@
         <v>575</v>
       </c>
       <c r="L6" t="s">
+        <v>591</v>
+      </c>
+      <c r="M6" t="s">
+        <v>592</v>
+      </c>
+      <c r="N6" t="s">
+        <v>591</v>
+      </c>
+      <c r="O6" t="s">
+        <v>667</v>
+      </c>
+      <c r="P6" t="s">
+        <v>668</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>667</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="U6" t="s">
         <v>593</v>
       </c>
-      <c r="M6" t="s">
+      <c r="V6" t="s">
         <v>594</v>
       </c>
-      <c r="N6" t="s">
-        <v>593</v>
-      </c>
-      <c r="O6" t="s">
-        <v>669</v>
-      </c>
-      <c r="P6" t="s">
-        <v>670</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>669</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>595</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>596</v>
-      </c>
-      <c r="W6" t="s">
-        <v>597</v>
-      </c>
-      <c r="X6" t="s">
-        <v>598</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="AA6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="AF6" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="AG6" s="3" t="s">
-        <v>585</v>
-      </c>
       <c r="AH6" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="AI6" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="AJ6" s="3" t="s">
         <v>565</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>
@@ -5952,13 +5952,13 @@
         <v>346</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
@@ -6147,10 +6147,10 @@
         <v>305</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>309</v>
@@ -6189,25 +6189,25 @@
         <v>341</v>
       </c>
       <c r="U4" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>721</v>
       </c>
-      <c r="V4" s="3" t="s">
-        <v>722</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>723</v>
-      </c>
       <c r="X4" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>220</v>
@@ -6255,13 +6255,13 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>603</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>604</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>605</v>
       </c>
       <c r="D6">
         <v>9606</v>
@@ -6279,28 +6279,28 @@
         <v>570</v>
       </c>
       <c r="I6" t="s">
+        <v>605</v>
+      </c>
+      <c r="J6" t="s">
+        <v>606</v>
+      </c>
+      <c r="K6" t="s">
         <v>607</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>608</v>
       </c>
-      <c r="K6" t="s">
-        <v>609</v>
-      </c>
-      <c r="L6" t="s">
-        <v>610</v>
-      </c>
       <c r="M6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="P6" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="Q6">
         <v>10</v>
@@ -6315,13 +6315,13 @@
         <v>575</v>
       </c>
       <c r="U6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="V6" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="W6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6330,19 +6330,19 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="AA6" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -6376,7 +6376,7 @@
         <v>355</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>357</v>
@@ -6400,22 +6400,22 @@
         <v>379</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>739</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
@@ -6444,13 +6444,13 @@
         <v>380</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>727</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="119" x14ac:dyDescent="0.2">
@@ -6479,13 +6479,13 @@
         <v>381</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -6496,7 +6496,7 @@
         <v>300</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>363</v>
@@ -6511,19 +6511,19 @@
         <v>375</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>382</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>730</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>732</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>435</v>
@@ -6532,7 +6532,7 @@
         <v>510</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6556,16 +6556,16 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="C6" t="s">
         <v>616</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>603</v>
-      </c>
-      <c r="C6" t="s">
-        <v>618</v>
-      </c>
       <c r="E6" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -6574,22 +6574,22 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -6597,16 +6597,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>615</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="C7" t="s">
+        <v>616</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>617</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>603</v>
-      </c>
-      <c r="C7" t="s">
-        <v>618</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>619</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -6615,22 +6615,22 @@
         <v>75</v>
       </c>
       <c r="H7" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -6778,13 +6778,13 @@
         <v>402</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>694</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>695</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6802,31 +6802,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>621</v>
+      </c>
+      <c r="B6" t="s">
+        <v>622</v>
+      </c>
+      <c r="C6" t="s">
         <v>623</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>624</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>625</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>626</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>627</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>628</v>
       </c>
-      <c r="G6" t="s">
-        <v>629</v>
-      </c>
-      <c r="H6" t="s">
-        <v>630</v>
-      </c>
       <c r="I6" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed development ontology to hsapdv for human donor
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karoly/dev/hca/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/HumanCellAtlas/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CE5370-08FB-6648-8E18-DB9E7B74BFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59138B0-0942-5E40-8BB1-752F633970CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-5940" windowWidth="51200" windowHeight="28340" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26700" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1782,12 +1782,6 @@
     <t>UO:0000036</t>
   </si>
   <si>
-    <t>adult</t>
-  </si>
-  <si>
-    <t>EFO:0001272</t>
-  </si>
-  <si>
     <t>days</t>
   </si>
   <si>
@@ -2293,6 +2287,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>human adult stage</t>
+  </si>
+  <si>
+    <t>HsapDv:0000087</t>
   </si>
 </sst>
 </file>
@@ -2770,7 +2770,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
@@ -2779,7 +2779,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2796,16 +2796,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>676</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2834,10 +2834,10 @@
         <v>536</v>
       </c>
       <c r="E6" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F6" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="G6" t="s">
         <v>538</v>
@@ -2974,13 +2974,13 @@
         <v>412</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>696</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2998,31 +2998,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B6" t="s">
+        <v>628</v>
+      </c>
+      <c r="C6" t="s">
+        <v>629</v>
+      </c>
+      <c r="D6" t="s">
+        <v>623</v>
+      </c>
+      <c r="E6" t="s">
+        <v>624</v>
+      </c>
+      <c r="F6" t="s">
+        <v>625</v>
+      </c>
+      <c r="G6" t="s">
+        <v>632</v>
+      </c>
+      <c r="H6" t="s">
         <v>630</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I6" t="s">
         <v>631</v>
-      </c>
-      <c r="D6" t="s">
-        <v>625</v>
-      </c>
-      <c r="E6" t="s">
-        <v>626</v>
-      </c>
-      <c r="F6" t="s">
-        <v>627</v>
-      </c>
-      <c r="G6" t="s">
-        <v>634</v>
-      </c>
-      <c r="H6" t="s">
-        <v>632</v>
-      </c>
-      <c r="I6" t="s">
-        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -3181,22 +3181,22 @@
         <v>421</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>715</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>717</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>428</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3217,34 +3217,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>634</v>
+      </c>
+      <c r="B6" t="s">
+        <v>635</v>
+      </c>
+      <c r="C6" t="s">
         <v>636</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>623</v>
+      </c>
+      <c r="E6" t="s">
+        <v>624</v>
+      </c>
+      <c r="F6" t="s">
+        <v>625</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="J6" t="s">
         <v>637</v>
-      </c>
-      <c r="C6" t="s">
-        <v>638</v>
-      </c>
-      <c r="D6" t="s">
-        <v>625</v>
-      </c>
-      <c r="E6" t="s">
-        <v>626</v>
-      </c>
-      <c r="F6" t="s">
-        <v>627</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="J6" t="s">
-        <v>639</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3325,13 +3325,13 @@
         <v>463</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>468</v>
@@ -3619,13 +3619,13 @@
         <v>466</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>471</v>
@@ -3711,84 +3711,84 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>641</v>
+      </c>
+      <c r="B6" t="s">
         <v>643</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>642</v>
+      </c>
+      <c r="D6" t="s">
+        <v>623</v>
+      </c>
+      <c r="E6" t="s">
+        <v>624</v>
+      </c>
+      <c r="F6" t="s">
+        <v>625</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="C6" t="s">
+      <c r="M6" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="D6" t="s">
-        <v>625</v>
-      </c>
-      <c r="E6" t="s">
-        <v>626</v>
-      </c>
-      <c r="F6" t="s">
-        <v>627</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>646</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>649</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>651</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="U6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X6" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="Y6">
         <v>20014279</v>
       </c>
       <c r="Z6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="AA6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
+        <v>652</v>
+      </c>
+      <c r="AD6" s="6" t="s">
         <v>654</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AE6" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>656</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>657</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>658</v>
       </c>
     </row>
   </sheetData>
@@ -3983,13 +3983,13 @@
         <v>530</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>699</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>700</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4012,46 +4012,46 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B6" t="s">
+        <v>657</v>
+      </c>
+      <c r="C6" t="s">
+        <v>658</v>
+      </c>
+      <c r="D6" t="s">
+        <v>623</v>
+      </c>
+      <c r="E6" t="s">
+        <v>624</v>
+      </c>
+      <c r="F6" t="s">
+        <v>625</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>659</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" s="3" t="s">
         <v>660</v>
       </c>
-      <c r="D6" t="s">
-        <v>625</v>
-      </c>
-      <c r="E6" t="s">
-        <v>626</v>
-      </c>
-      <c r="F6" t="s">
-        <v>627</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="J6" t="s">
         <v>661</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>661</v>
-      </c>
-      <c r="J6" t="s">
-        <v>663</v>
       </c>
       <c r="K6" t="s">
         <v>553</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
   </sheetData>
@@ -4172,7 +4172,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
@@ -4196,7 +4196,7 @@
         <v>57</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>64</v>
@@ -4320,7 +4320,7 @@
         <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4340,7 +4340,7 @@
         <v>81</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4360,7 +4360,7 @@
         <v>82</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4368,7 +4368,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>75</v>
@@ -4377,10 +4377,10 @@
         <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4410,7 +4410,7 @@
         <v>561</v>
       </c>
       <c r="F6" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
   </sheetData>
@@ -4475,7 +4475,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4505,8 +4505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4971,10 +4971,10 @@
         <v>113</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>123</v>
@@ -5195,58 +5195,58 @@
         <v>578</v>
       </c>
       <c r="V6" t="s">
-        <v>580</v>
+        <v>749</v>
       </c>
       <c r="W6" t="s">
-        <v>581</v>
+        <v>750</v>
       </c>
       <c r="X6" t="s">
-        <v>580</v>
+        <v>749</v>
       </c>
       <c r="Y6" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="Z6" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="AA6" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
+        <v>580</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="AE6" t="s">
         <v>582</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>584</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="AH6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="AI6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="AL6" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="AM6" t="s">
         <v>587</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -5627,10 +5627,10 @@
         <v>225</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>227</v>
@@ -5651,13 +5651,13 @@
         <v>238</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>688</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>689</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>690</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>244</v>
@@ -5675,7 +5675,7 @@
         <v>255</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>262</v>
@@ -5687,7 +5687,7 @@
         <v>270</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>277</v>
@@ -5763,13 +5763,13 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D6">
         <v>9606</v>
@@ -5793,82 +5793,82 @@
         <v>574</v>
       </c>
       <c r="L6" t="s">
+        <v>590</v>
+      </c>
+      <c r="M6" t="s">
+        <v>591</v>
+      </c>
+      <c r="N6" t="s">
+        <v>590</v>
+      </c>
+      <c r="O6" t="s">
+        <v>666</v>
+      </c>
+      <c r="P6" t="s">
+        <v>667</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>666</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="U6" t="s">
         <v>592</v>
       </c>
-      <c r="M6" t="s">
+      <c r="V6" t="s">
         <v>593</v>
       </c>
-      <c r="N6" t="s">
-        <v>592</v>
-      </c>
-      <c r="O6" t="s">
-        <v>668</v>
-      </c>
-      <c r="P6" t="s">
-        <v>669</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>668</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>594</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>595</v>
-      </c>
-      <c r="W6" t="s">
-        <v>596</v>
-      </c>
-      <c r="X6" t="s">
-        <v>597</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="AA6" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="AF6" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="AG6" s="3" t="s">
-        <v>584</v>
-      </c>
       <c r="AH6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="AI6" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="AJ6" s="3" t="s">
         <v>565</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -5880,7 +5880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -5976,13 +5976,13 @@
         <v>346</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
@@ -6171,10 +6171,10 @@
         <v>305</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>309</v>
@@ -6213,25 +6213,25 @@
         <v>341</v>
       </c>
       <c r="U4" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>720</v>
       </c>
-      <c r="V4" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>722</v>
-      </c>
       <c r="X4" s="3" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>220</v>
@@ -6279,13 +6279,13 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>602</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>603</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>604</v>
       </c>
       <c r="D6">
         <v>9606</v>
@@ -6300,28 +6300,28 @@
         <v>569</v>
       </c>
       <c r="I6" t="s">
+        <v>604</v>
+      </c>
+      <c r="J6" t="s">
+        <v>605</v>
+      </c>
+      <c r="K6" t="s">
         <v>606</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>607</v>
       </c>
-      <c r="K6" t="s">
-        <v>608</v>
-      </c>
-      <c r="L6" t="s">
-        <v>609</v>
-      </c>
       <c r="M6" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="P6" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="Q6">
         <v>10</v>
@@ -6336,13 +6336,13 @@
         <v>574</v>
       </c>
       <c r="U6" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="V6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="W6" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6351,19 +6351,19 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="AA6" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -6397,7 +6397,7 @@
         <v>355</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>357</v>
@@ -6421,22 +6421,22 @@
         <v>379</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>738</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
@@ -6465,13 +6465,13 @@
         <v>380</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>726</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="119" x14ac:dyDescent="0.2">
@@ -6500,13 +6500,13 @@
         <v>381</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -6517,7 +6517,7 @@
         <v>300</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>363</v>
@@ -6532,19 +6532,19 @@
         <v>375</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>382</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>729</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>731</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>435</v>
@@ -6553,7 +6553,7 @@
         <v>510</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6577,16 +6577,16 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>613</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="C6" t="s">
         <v>615</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="C6" t="s">
-        <v>617</v>
-      </c>
       <c r="E6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -6595,22 +6595,22 @@
         <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -6618,16 +6618,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>614</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="C7" t="s">
+        <v>615</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>616</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="C7" t="s">
-        <v>617</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>618</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -6636,22 +6636,22 @@
         <v>75</v>
       </c>
       <c r="H7" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -6799,13 +6799,13 @@
         <v>402</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>693</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>694</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6823,31 +6823,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B6" t="s">
+        <v>621</v>
+      </c>
+      <c r="C6" t="s">
         <v>622</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>623</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>624</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>625</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>626</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>627</v>
       </c>
-      <c r="G6" t="s">
-        <v>628</v>
-      </c>
-      <c r="H6" t="s">
-        <v>629</v>
-      </c>
       <c r="I6" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change system tests spreadsheet ontology terms from data:3494 to EDAM:3494. Fixes #1757
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1610,7 +1610,7 @@
     <t>For example: DNA sequence (raw); Sequence alignment</t>
   </si>
   <si>
-    <t>For example: DATA:3497; DATA:0863</t>
+    <t>For example: EDAM:3497; EDAM:0863</t>
   </si>
   <si>
     <t>sequence_file.file_core.file_name</t>
@@ -1670,7 +1670,7 @@
     <t>DNA sequence</t>
   </si>
   <si>
-    <t>data:3494</t>
+    <t>EDAM:3494</t>
   </si>
   <si>
     <t>lib_prep_1</t>
@@ -2502,7 +2502,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -2533,10 +2533,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2551,10 +2551,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2566,19 +2566,19 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2590,19 +2590,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2617,10 +2611,10 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2799,9 +2793,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -2881,7 +2875,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2908,10 +2902,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3158,9 +3152,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -3438,7 +3432,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3465,10 +3459,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3949,11 +3943,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="25.6719" style="35" customWidth="1"/>
-    <col min="7" max="7" width="57.6719" style="35" customWidth="1"/>
-    <col min="8" max="8" width="50.6719" style="35" customWidth="1"/>
-    <col min="9" max="9" width="56.6719" style="35" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="35" customWidth="1"/>
+    <col min="1" max="6" width="25.6719" style="33" customWidth="1"/>
+    <col min="7" max="7" width="57.6719" style="33" customWidth="1"/>
+    <col min="8" max="8" width="50.6719" style="33" customWidth="1"/>
+    <col min="9" max="9" width="56.6719" style="33" customWidth="1"/>
+    <col min="10" max="16384" width="8.85156" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -4175,12 +4169,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="25.6719" style="36" customWidth="1"/>
-    <col min="7" max="7" width="53.6719" style="36" customWidth="1"/>
-    <col min="8" max="8" width="46.6719" style="36" customWidth="1"/>
-    <col min="9" max="9" width="52.6719" style="36" customWidth="1"/>
-    <col min="10" max="12" width="25.6719" style="36" customWidth="1"/>
-    <col min="13" max="16384" width="8.85156" style="36" customWidth="1"/>
+    <col min="1" max="6" width="25.6719" style="34" customWidth="1"/>
+    <col min="7" max="7" width="53.6719" style="34" customWidth="1"/>
+    <col min="8" max="8" width="46.6719" style="34" customWidth="1"/>
+    <col min="9" max="9" width="52.6719" style="34" customWidth="1"/>
+    <col min="10" max="12" width="25.6719" style="34" customWidth="1"/>
+    <col min="13" max="16384" width="8.85156" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -4462,18 +4456,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="25.6719" style="37" customWidth="1"/>
-    <col min="7" max="7" width="34.6719" style="37" customWidth="1"/>
-    <col min="8" max="10" width="25.6719" style="37" customWidth="1"/>
-    <col min="11" max="11" width="51.6719" style="37" customWidth="1"/>
-    <col min="12" max="12" width="65.6719" style="37" customWidth="1"/>
-    <col min="13" max="13" width="71.6719" style="37" customWidth="1"/>
-    <col min="14" max="14" width="25.6719" style="37" customWidth="1"/>
-    <col min="15" max="15" width="74.6719" style="37" customWidth="1"/>
-    <col min="16" max="16" width="67.6719" style="37" customWidth="1"/>
-    <col min="17" max="17" width="73.6719" style="37" customWidth="1"/>
-    <col min="18" max="32" width="25.6719" style="37" customWidth="1"/>
-    <col min="33" max="16384" width="8.85156" style="37" customWidth="1"/>
+    <col min="1" max="6" width="25.6719" style="35" customWidth="1"/>
+    <col min="7" max="7" width="34.6719" style="35" customWidth="1"/>
+    <col min="8" max="10" width="25.6719" style="35" customWidth="1"/>
+    <col min="11" max="11" width="51.6719" style="35" customWidth="1"/>
+    <col min="12" max="12" width="65.6719" style="35" customWidth="1"/>
+    <col min="13" max="13" width="71.6719" style="35" customWidth="1"/>
+    <col min="14" max="14" width="25.6719" style="35" customWidth="1"/>
+    <col min="15" max="15" width="74.6719" style="35" customWidth="1"/>
+    <col min="16" max="16" width="67.6719" style="35" customWidth="1"/>
+    <col min="17" max="17" width="73.6719" style="35" customWidth="1"/>
+    <col min="18" max="32" width="25.6719" style="35" customWidth="1"/>
+    <col min="33" max="16384" width="8.85156" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -4976,11 +4970,11 @@
       <c r="AA6" t="s" s="16">
         <v>715</v>
       </c>
-      <c r="AB6" s="38"/>
+      <c r="AB6" s="36"/>
       <c r="AC6" t="s" s="16">
         <v>716</v>
       </c>
-      <c r="AD6" t="s" s="39">
+      <c r="AD6" t="s" s="37">
         <v>718</v>
       </c>
       <c r="AE6" t="s" s="16">
@@ -5143,15 +5137,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="25.6719" style="40" customWidth="1"/>
-    <col min="7" max="7" width="65.6719" style="40" customWidth="1"/>
-    <col min="8" max="8" width="58.6719" style="40" customWidth="1"/>
-    <col min="9" max="9" width="64.6719" style="40" customWidth="1"/>
-    <col min="10" max="11" width="25.6719" style="40" customWidth="1"/>
-    <col min="12" max="12" width="55.6719" style="40" customWidth="1"/>
-    <col min="13" max="13" width="48.6719" style="40" customWidth="1"/>
-    <col min="14" max="14" width="54.6719" style="40" customWidth="1"/>
-    <col min="15" max="16384" width="8.85156" style="40" customWidth="1"/>
+    <col min="1" max="6" width="25.6719" style="38" customWidth="1"/>
+    <col min="7" max="7" width="65.6719" style="38" customWidth="1"/>
+    <col min="8" max="8" width="58.6719" style="38" customWidth="1"/>
+    <col min="9" max="9" width="64.6719" style="38" customWidth="1"/>
+    <col min="10" max="11" width="25.6719" style="38" customWidth="1"/>
+    <col min="12" max="12" width="55.6719" style="38" customWidth="1"/>
+    <col min="13" max="13" width="48.6719" style="38" customWidth="1"/>
+    <col min="14" max="14" width="54.6719" style="38" customWidth="1"/>
+    <col min="15" max="16384" width="8.85156" style="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -8583,13 +8577,13 @@
       <c r="I4" t="s" s="10">
         <v>531</v>
       </c>
-      <c r="J4" t="s" s="29">
+      <c r="J4" t="s" s="10">
         <v>532</v>
       </c>
-      <c r="K4" t="s" s="29">
+      <c r="K4" t="s" s="10">
         <v>533</v>
       </c>
-      <c r="L4" t="s" s="29">
+      <c r="L4" t="s" s="10">
         <v>534</v>
       </c>
       <c r="M4" t="s" s="10">
@@ -8649,13 +8643,13 @@
         <v>541</v>
       </c>
       <c r="I6" s="25"/>
-      <c r="J6" t="s" s="30">
+      <c r="J6" t="s" s="29">
         <v>542</v>
       </c>
-      <c r="K6" t="s" s="30">
+      <c r="K6" t="s" s="29">
         <v>543</v>
       </c>
-      <c r="L6" t="s" s="30">
+      <c r="L6" t="s" s="29">
         <v>542</v>
       </c>
       <c r="M6" t="s" s="16">
@@ -8684,23 +8678,23 @@
       <c r="E7" t="s" s="11">
         <v>547</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="30">
         <v>1</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="30">
         <v>75</v>
       </c>
       <c r="H7" t="s" s="11">
         <v>541</v>
       </c>
       <c r="I7" s="17"/>
-      <c r="J7" t="s" s="32">
+      <c r="J7" t="s" s="31">
         <v>542</v>
       </c>
-      <c r="K7" t="s" s="32">
+      <c r="K7" t="s" s="31">
         <v>543</v>
       </c>
-      <c r="L7" t="s" s="32">
+      <c r="L7" t="s" s="31">
         <v>542</v>
       </c>
       <c r="M7" t="s" s="11">
@@ -8709,7 +8703,7 @@
       <c r="N7" t="s" s="11">
         <v>545</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O7" s="30">
         <v>1</v>
       </c>
       <c r="P7" s="17"/>
@@ -8725,9 +8719,9 @@
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
@@ -8744,9 +8738,9 @@
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
@@ -8763,9 +8757,9 @@
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
@@ -8782,9 +8776,9 @@
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
@@ -8808,11 +8802,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="25.6719" style="34" customWidth="1"/>
-    <col min="7" max="7" width="53.6719" style="34" customWidth="1"/>
-    <col min="8" max="8" width="46.6719" style="34" customWidth="1"/>
-    <col min="9" max="9" width="52.6719" style="34" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="34" customWidth="1"/>
+    <col min="1" max="6" width="25.6719" style="32" customWidth="1"/>
+    <col min="7" max="7" width="53.6719" style="32" customWidth="1"/>
+    <col min="8" max="8" width="46.6719" style="32" customWidth="1"/>
+    <col min="9" max="9" width="52.6719" style="32" customWidth="1"/>
+    <col min="10" max="16384" width="8.85156" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">

</xml_diff>